<commit_message>
Added a second wave to the tutorial. Heroes now keep their HP and Mana between waves. The Intro now transitions to the tutorial. Skip intro with Escape
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="12345" activeTab="1"/>
+    <workbookView windowWidth="26715" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,6 @@
   </si>
   <si>
     <t>Suzanna Heals 5
-Big Boyo has Armor 1
 Lil Munchy has 3 - 4</t>
   </si>
   <si>
@@ -485,10 +484,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -546,6 +545,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -554,7 +568,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -570,22 +615,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -595,30 +625,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -648,21 +654,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -699,13 +698,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,7 +722,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,13 +770,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,73 +812,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,13 +836,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,31 +854,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1129,11 +1128,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1149,15 +1161,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1179,9 +1182,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1201,17 +1206,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1229,7 +1228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1247,130 +1246,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1837,8 +1836,8 @@
   <sheetPr/>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -2598,8 +2597,8 @@
   <sheetPr/>
   <dimension ref="A3:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>

</xml_diff>

<commit_message>
Added mana bars to units (should work properly). Also added mana costs to spells. Normalized the first 2 encounters. Made some more items.
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26715" windowHeight="12345"/>
+    <workbookView windowWidth="13935" windowHeight="12945" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,10 @@
     <t>13</t>
   </si>
   <si>
-    <t>Prison Guard</t>
+    <t>Town Guard</t>
+  </si>
+  <si>
+    <t>1 - 2</t>
   </si>
   <si>
     <t>Armor 1</t>
@@ -169,9 +172,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>1 - 2</t>
-  </si>
-  <si>
     <t>On death, leaves spikes
 on the ground
 (2 damage)</t>
@@ -189,7 +189,7 @@
     <t>Heal 6</t>
   </si>
   <si>
-    <t>Town Guard</t>
+    <t>Prison Guard</t>
   </si>
   <si>
     <t>16</t>
@@ -484,10 +484,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -546,15 +546,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -568,15 +568,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -585,13 +577,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -606,18 +591,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -660,15 +637,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -683,7 +668,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -698,7 +698,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,25 +716,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -746,7 +740,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,13 +752,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,25 +782,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,7 +806,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,31 +854,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -860,25 +872,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1122,30 +1122,6 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1161,6 +1137,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1182,11 +1167,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1206,11 +1189,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1223,20 +1212,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1246,130 +1246,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1836,7 +1836,7 @@
   <sheetPr/>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -2597,8 +2597,8 @@
   <sheetPr/>
   <dimension ref="A3:N34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -2673,91 +2673,91 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N6" s="8"/>
     </row>
     <row r="7" ht="75" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N7" s="8"/>
     </row>
     <row r="8" ht="37.5" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N8" s="8"/>
     </row>
     <row r="9" ht="75" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>50</v>
@@ -2769,7 +2769,7 @@
         <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>52</v>
@@ -2787,7 +2787,7 @@
         <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>56</v>
@@ -2805,10 +2805,10 @@
         <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>59</v>
@@ -2817,7 +2817,7 @@
         <v>60</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>61</v>
@@ -2850,7 +2850,7 @@
         <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>63</v>
@@ -2931,7 +2931,7 @@
         <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>63</v>
@@ -3023,7 +3023,7 @@
         <v>102</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>89</v>
@@ -3061,7 +3061,7 @@
         <v>109</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>8</v>
@@ -3107,7 +3107,7 @@
         <v>114</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>108</v>
@@ -3252,7 +3252,7 @@
         <v>134</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K30" s="12">
         <v>7</v>

</xml_diff>

<commit_message>
Made Ranger Rescue Mission. Remade the tutorial and now it works with the new events system. Made Little Scout and Scrub Scout.
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13935" windowHeight="12945" activeTab="1"/>
+    <workbookView windowWidth="27870" windowHeight="13095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="139">
   <si>
     <t>Player Level</t>
   </si>
@@ -104,16 +104,13 @@
     <t>1</t>
   </si>
   <si>
-    <t>13</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>1 - 2</t>
   </si>
   <si>
     <t>Town Guard</t>
-  </si>
-  <si>
-    <t>1 - 2</t>
-  </si>
-  <si>
-    <t>Armor 1</t>
   </si>
   <si>
     <t>Serfmaster</t>
@@ -545,9 +542,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,23 +556,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -591,10 +596,32 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -629,11 +656,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -646,14 +672,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -662,28 +681,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -698,7 +695,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,7 +809,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,67 +833,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,73 +851,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -878,7 +863,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1122,6 +1119,26 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1165,6 +1182,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1188,47 +1220,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1246,130 +1243,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2598,7 +2595,7 @@
   <dimension ref="A3:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -2658,13 +2655,13 @@
         <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -2673,395 +2670,393 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N6" s="8"/>
     </row>
     <row r="7" ht="75" spans="1:14">
       <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="N7" s="8"/>
     </row>
     <row r="8" ht="37.5" spans="1:14">
       <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="N8" s="8"/>
     </row>
     <row r="9" ht="75" spans="1:14">
       <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="N9" s="8"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N11" s="8"/>
     </row>
     <row r="12" ht="56.25" spans="1:14">
       <c r="A12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="N12" s="8"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="N13" s="8"/>
     </row>
     <row r="14" ht="37.5" spans="1:14">
       <c r="A14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="H14" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="N14" s="9"/>
     </row>
     <row r="15" ht="56.25" spans="1:7">
       <c r="A15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" ht="56.25" spans="1:6">
       <c r="A17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" ht="93.75" spans="1:8">
       <c r="A18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" ht="37.5" spans="1:8">
       <c r="A19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="H19" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="20" ht="37.5" spans="1:8">
       <c r="A20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>97</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" ht="37.5" spans="1:7">
       <c r="A21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="22" ht="56.25" spans="1:8">
       <c r="A22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="23" ht="37.5" spans="1:13">
       <c r="A23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>8</v>
@@ -3075,22 +3070,22 @@
     </row>
     <row r="24" ht="56.25" spans="1:13">
       <c r="A24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="K24" s="12">
         <v>1</v>
@@ -3104,28 +3099,28 @@
     </row>
     <row r="25" ht="37.5" spans="1:13">
       <c r="A25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="K25" s="12">
         <v>2</v>
@@ -3139,19 +3134,19 @@
     </row>
     <row r="26" ht="37.5" spans="1:13">
       <c r="A26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="K26" s="12">
         <v>3</v>
@@ -3165,19 +3160,19 @@
     </row>
     <row r="27" ht="56.25" spans="1:13">
       <c r="A27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="K27" s="12">
         <v>4</v>
@@ -3191,25 +3186,25 @@
     </row>
     <row r="28" ht="37.5" spans="1:13">
       <c r="A28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="G28" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="K28" s="12">
         <v>5</v>
@@ -3223,19 +3218,19 @@
     </row>
     <row r="29" ht="37.5" spans="1:13">
       <c r="A29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K29" s="12">
         <v>6</v>
@@ -3249,10 +3244,10 @@
     </row>
     <row r="30" ht="37.5" spans="1:13">
       <c r="A30" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K30" s="12">
         <v>7</v>
@@ -3266,7 +3261,7 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K31" s="12">
         <v>8</v>
@@ -3280,10 +3275,10 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="K32" s="12">
         <v>9</v>
@@ -3297,10 +3292,10 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K33" s="14">
         <v>10</v>
@@ -3314,10 +3309,10 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Hay Added Gravestone. Added Triple Arrow spell for Ranger (and its tome). Added Forks and Candles encounter (with a Bishop).
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -223,11 +223,141 @@
       </xdr:spPr>
     </xdr:pic>
   </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="ID_CC66E0BDF222479FBCA1D73D9EEF98C9" descr="Log"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9"/>
+        <a:srcRect l="21573" t="62476" r="20720"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7954645" y="2811780"/>
+          <a:ext cx="1160780" cy="368935"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="ID_DD37BC4AF6A646D482F166D1DA3483B9" descr="Table"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId10"/>
+        <a:srcRect l="25413" t="47320" r="22391"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8062595" y="3523615"/>
+          <a:ext cx="903605" cy="410210"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="ID_03A246FAB8D54EF0A611A5197A16854B" descr="gravestone"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId11"/>
+        <a:srcRect l="27241" t="19165" r="21981"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8237855" y="2737485"/>
+          <a:ext cx="462915" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="ID_69F91952F7254C9081725FDDC3777D6A" descr="bush"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId12"/>
+        <a:srcRect l="27254" t="68910" r="24803"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8087360" y="4425950"/>
+          <a:ext cx="440055" cy="282575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="ID_5883AB3B095E4C91BA3FA08ED96F1A98" descr="hay"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId13"/>
+        <a:srcRect l="11806" t="45540" r="9444"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8113395" y="5283200"/>
+          <a:ext cx="720090" cy="490855"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
 </etc:cellImages>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
   <si>
     <t>Player Level</t>
   </si>
@@ -703,7 +833,20 @@
     <t>Bear Trap</t>
   </si>
   <si>
-    <t>On step: damage</t>
+    <r>
+      <t>Step</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: damage,
+then it disappears</t>
+    </r>
   </si>
   <si>
     <t>Barrel</t>
@@ -712,19 +855,46 @@
     <t>Spikes</t>
   </si>
   <si>
-    <t>On step: damage
+    <r>
+      <t>Step</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: damage
 Toggles at round end</t>
+    </r>
   </si>
   <si>
     <t>Crate</t>
+  </si>
+  <si>
+    <t>Small chance
+to drop loot</t>
   </si>
   <si>
     <t>Explosive
 Barrel</t>
   </si>
   <si>
-    <t>Explodes [square]
-on death</t>
+    <r>
+      <t>Death</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Explodes [square]</t>
+    </r>
   </si>
   <si>
     <t>Rocks</t>
@@ -733,11 +903,61 @@
     <t>Poison Vase</t>
   </si>
   <si>
-    <t>Leaves acid around
+    <r>
+      <t>Death</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Leaves acid around
 [square]</t>
+    </r>
+  </si>
+  <si>
+    <t>Gravestone</t>
+  </si>
+  <si>
+    <t>Small chance
+to drop zombie</t>
   </si>
   <si>
     <t>Acid</t>
+  </si>
+  <si>
+    <r>
+      <t>Step</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: damage</t>
+    </r>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Log</t>
+  </si>
+  <si>
+    <t>Bush</t>
+  </si>
+  <si>
+    <t>Hay</t>
+  </si>
+  <si>
+    <t>Small chance
+to drop child</t>
   </si>
 </sst>
 </file>
@@ -745,12 +965,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -769,6 +989,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.25"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -806,9 +1033,115 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -823,39 +1156,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -866,85 +1170,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -959,13 +1186,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -983,13 +1204,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1007,73 +1312,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1085,7 +1324,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1103,43 +1342,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1383,26 +1610,6 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1422,15 +1629,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1442,6 +1640,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1463,9 +1670,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1484,12 +1693,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1507,130 +1734,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1644,8 +1871,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1653,9 +1883,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1663,6 +1890,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1695,10 +1925,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1761,7 +1988,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2112,31 +2339,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="18.7142857142857" style="19" customWidth="1"/>
-    <col min="2" max="2" width="20.4285714285714" style="19" customWidth="1"/>
-    <col min="3" max="3" width="9.71428571428571" style="19" customWidth="1"/>
-    <col min="4" max="4" width="11.1428571428571" style="19" customWidth="1"/>
-    <col min="5" max="5" width="13.7142857142857" style="19" customWidth="1"/>
-    <col min="6" max="6" width="17.7142857142857" style="19" customWidth="1"/>
-    <col min="7" max="7" width="17.8571428571429" style="19" customWidth="1"/>
-    <col min="8" max="8" width="17.5714285714286" style="19" customWidth="1"/>
-    <col min="9" max="9" width="19.1428571428571" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="9.14285714285714" style="19"/>
+    <col min="1" max="1" width="18.7142857142857" style="20" customWidth="1"/>
+    <col min="2" max="2" width="20.4285714285714" style="20" customWidth="1"/>
+    <col min="3" max="3" width="9.71428571428571" style="20" customWidth="1"/>
+    <col min="4" max="4" width="11.1428571428571" style="20" customWidth="1"/>
+    <col min="5" max="5" width="13.7142857142857" style="20" customWidth="1"/>
+    <col min="6" max="6" width="17.7142857142857" style="20" customWidth="1"/>
+    <col min="7" max="7" width="17.8571428571429" style="20" customWidth="1"/>
+    <col min="8" max="8" width="17.5714285714286" style="20" customWidth="1"/>
+    <col min="9" max="9" width="19.1428571428571" style="20" customWidth="1"/>
+    <col min="10" max="16384" width="9.14285714285714" style="20"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:9">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="20"/>
+      <c r="A2" s="1"/>
       <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
@@ -2161,12 +2388,12 @@
       <c r="I2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="20"/>
+      <c r="A3" s="1"/>
       <c r="B3" s="28">
         <v>1</v>
       </c>
@@ -2193,7 +2420,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="20"/>
+      <c r="A4" s="1"/>
       <c r="B4" s="28">
         <v>2</v>
       </c>
@@ -2209,7 +2436,7 @@
       <c r="F4" s="35">
         <v>9</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="1">
         <v>9</v>
       </c>
       <c r="H4" s="36">
@@ -2220,7 +2447,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="20"/>
+      <c r="A5" s="1"/>
       <c r="B5" s="28">
         <v>3</v>
       </c>
@@ -2247,7 +2474,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="20"/>
+      <c r="A6" s="1"/>
       <c r="B6" s="28">
         <v>4</v>
       </c>
@@ -2263,7 +2490,7 @@
       <c r="F6" s="35">
         <v>14</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="1">
         <v>14</v>
       </c>
       <c r="H6" s="36">
@@ -2274,7 +2501,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="20"/>
+      <c r="A7" s="1"/>
       <c r="B7" s="28">
         <v>5</v>
       </c>
@@ -2301,7 +2528,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="20"/>
+      <c r="A8" s="1"/>
       <c r="B8" s="28">
         <v>6</v>
       </c>
@@ -2317,7 +2544,7 @@
       <c r="F8" s="35">
         <v>19</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="1">
         <v>19</v>
       </c>
       <c r="H8" s="36">
@@ -2328,7 +2555,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="20"/>
+      <c r="A9" s="1"/>
       <c r="B9" s="28">
         <v>7</v>
       </c>
@@ -2355,7 +2582,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="20"/>
+      <c r="A10" s="1"/>
       <c r="B10" s="28">
         <v>8</v>
       </c>
@@ -2371,7 +2598,7 @@
       <c r="F10" s="35">
         <v>24</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="1">
         <v>24</v>
       </c>
       <c r="H10" s="36">
@@ -2382,7 +2609,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="20"/>
+      <c r="A11" s="1"/>
       <c r="B11" s="28">
         <v>9</v>
       </c>
@@ -2409,7 +2636,7 @@
       </c>
     </row>
     <row r="12" ht="19.5" spans="1:9">
-      <c r="A12" s="20"/>
+      <c r="A12" s="1"/>
       <c r="B12" s="37">
         <v>10</v>
       </c>
@@ -2436,40 +2663,40 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="20"/>
+      <c r="A16" s="1"/>
       <c r="B16" s="42" t="s">
         <v>8</v>
       </c>
@@ -2485,17 +2712,17 @@
       <c r="F16" s="45"/>
       <c r="G16" s="46"/>
       <c r="H16" s="47"/>
-      <c r="I16" s="20"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="20"/>
+      <c r="A17" s="1"/>
       <c r="B17" s="28">
         <v>1</v>
       </c>
       <c r="C17" s="34">
         <v>15</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="36">
@@ -2504,17 +2731,17 @@
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
       <c r="H17" s="47"/>
-      <c r="I17" s="20"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="20"/>
+      <c r="A18" s="1"/>
       <c r="B18" s="28">
         <v>2</v>
       </c>
       <c r="C18" s="36">
         <v>21</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="36">
@@ -2523,17 +2750,17 @@
       <c r="F18" s="47"/>
       <c r="G18" s="47"/>
       <c r="H18" s="47"/>
-      <c r="I18" s="20"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="20"/>
+      <c r="A19" s="1"/>
       <c r="B19" s="28">
         <v>3</v>
       </c>
       <c r="C19" s="36">
         <v>27</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="36">
@@ -2542,17 +2769,17 @@
       <c r="F19" s="47"/>
       <c r="G19" s="47"/>
       <c r="H19" s="47"/>
-      <c r="I19" s="20"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="20"/>
+      <c r="A20" s="1"/>
       <c r="B20" s="28">
         <v>4</v>
       </c>
       <c r="C20" s="36">
         <v>33</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="36">
@@ -2561,17 +2788,17 @@
       <c r="F20" s="47"/>
       <c r="G20" s="47"/>
       <c r="H20" s="47"/>
-      <c r="I20" s="20"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="20"/>
+      <c r="A21" s="1"/>
       <c r="B21" s="28">
         <v>5</v>
       </c>
       <c r="C21" s="36">
         <v>39</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="36">
@@ -2580,7 +2807,7 @@
       <c r="F21" s="47"/>
       <c r="G21" s="47"/>
       <c r="H21" s="47"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="28">
@@ -2589,7 +2816,7 @@
       <c r="C22" s="36">
         <v>45</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="36">
@@ -2606,7 +2833,7 @@
       <c r="C23" s="36">
         <v>51</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="36">
@@ -2623,7 +2850,7 @@
       <c r="C24" s="36">
         <v>57</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="36">
@@ -2640,7 +2867,7 @@
       <c r="C25" s="36">
         <v>63</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="36">
@@ -2657,7 +2884,7 @@
       <c r="C26" s="41">
         <v>69</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="19" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="41">
@@ -2686,175 +2913,175 @@
       <c r="H31"/>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:8">
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" spans="2:8">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" spans="2:8">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" spans="2:8">
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" spans="2:8">
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
     </row>
     <row r="39" spans="2:8">
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
     </row>
     <row r="40" spans="2:8">
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41" spans="2:8">
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" spans="2:8">
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
     </row>
     <row r="43" spans="2:8">
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
     </row>
     <row r="44" spans="2:8">
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" spans="2:8">
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" spans="2:8">
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" spans="2:8">
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="48" spans="2:8">
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2873,21 +3100,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="21.1428571428571" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.5714285714286" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.42857142857143" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.5714285714286" style="5" customWidth="1"/>
-    <col min="5" max="5" width="17.8571428571429" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26" style="5" customWidth="1"/>
-    <col min="7" max="7" width="27" style="5" customWidth="1"/>
-    <col min="8" max="8" width="16.8571428571429" style="5" customWidth="1"/>
-    <col min="9" max="9" width="5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="2.57142857142857" style="5" customWidth="1"/>
-    <col min="11" max="11" width="18.5714285714286" style="5" customWidth="1"/>
-    <col min="12" max="12" width="9.14285714285714" style="5"/>
-    <col min="13" max="13" width="11.5714285714286" style="5" customWidth="1"/>
-    <col min="14" max="14" width="13.4285714285714" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="9.14285714285714" style="5"/>
+    <col min="1" max="1" width="21.1428571428571" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.5714285714286" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.42857142857143" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.5714285714286" style="6" customWidth="1"/>
+    <col min="5" max="5" width="17.8571428571429" style="6" customWidth="1"/>
+    <col min="6" max="6" width="26" style="6" customWidth="1"/>
+    <col min="7" max="7" width="27" style="6" customWidth="1"/>
+    <col min="8" max="8" width="16.8571428571429" style="6" customWidth="1"/>
+    <col min="9" max="9" width="5" style="6" customWidth="1"/>
+    <col min="10" max="10" width="2.57142857142857" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.5714285714286" style="6" customWidth="1"/>
+    <col min="12" max="12" width="9.14285714285714" style="6"/>
+    <col min="13" max="13" width="11.5714285714286" style="6" customWidth="1"/>
+    <col min="14" max="14" width="13.4285714285714" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="9.14285714285714" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="14:14">
@@ -2900,694 +3127,694 @@
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>26</v>
       </c>
       <c r="N3"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="N4"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>12</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="N5"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="N6"/>
     </row>
     <row r="7" ht="75" spans="1:14">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="11" t="s">
         <v>40</v>
       </c>
       <c r="N7"/>
     </row>
     <row r="8" ht="37.5" spans="1:14">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>45</v>
       </c>
       <c r="N8"/>
     </row>
     <row r="9" ht="75" spans="1:14">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="11" t="s">
         <v>49</v>
       </c>
       <c r="N9"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="6" t="s">
         <v>53</v>
       </c>
       <c r="N10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="6" t="s">
         <v>56</v>
       </c>
       <c r="N11"/>
     </row>
     <row r="12" ht="56.25" spans="1:14">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="11" t="s">
         <v>60</v>
       </c>
       <c r="N12"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="6" t="s">
         <v>65</v>
       </c>
       <c r="N13"/>
     </row>
     <row r="14" ht="37.5" spans="1:14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="11" t="s">
         <v>70</v>
       </c>
       <c r="N14"/>
     </row>
     <row r="15" ht="56.25" spans="1:14">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="11" t="s">
         <v>74</v>
       </c>
       <c r="N15"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" ht="56.25" spans="1:6">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="11" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="18" ht="93.75" spans="1:8">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="11" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="19" ht="37.5" spans="1:8">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="20" ht="37.5" spans="1:8">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="21" ht="37.5" spans="1:7">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="22" ht="56.25" spans="1:8">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="11" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="23" ht="37.5" spans="1:13">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="K23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L23" s="11" t="s">
+      <c r="L23" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M23" s="12" t="s">
+      <c r="M23" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" ht="56.25" spans="1:13">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="14">
         <v>1</v>
       </c>
-      <c r="L24" s="14">
+      <c r="L24" s="15">
         <v>15</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="M24" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" ht="37.5" spans="1:13">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="K25" s="13">
+      <c r="K25" s="14">
         <v>2</v>
       </c>
-      <c r="L25" s="15">
+      <c r="L25" s="16">
         <v>21</v>
       </c>
-      <c r="M25" s="5" t="s">
+      <c r="M25" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" ht="37.5" spans="1:13">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="K26" s="13">
+      <c r="K26" s="14">
         <v>3</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L26" s="16">
         <v>27</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="M26" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" ht="56.25" spans="1:13">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="K27" s="13">
+      <c r="K27" s="14">
         <v>4</v>
       </c>
-      <c r="L27" s="15">
+      <c r="L27" s="16">
         <v>33</v>
       </c>
-      <c r="M27" s="5" t="s">
+      <c r="M27" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="28" ht="37.5" spans="1:13">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="K28" s="13">
+      <c r="K28" s="14">
         <v>5</v>
       </c>
-      <c r="L28" s="15">
+      <c r="L28" s="16">
         <v>39</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="M28" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" ht="37.5" spans="1:13">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="K29" s="13">
+      <c r="K29" s="14">
         <v>6</v>
       </c>
-      <c r="L29" s="15">
+      <c r="L29" s="16">
         <v>45</v>
       </c>
-      <c r="M29" s="5" t="s">
+      <c r="M29" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" ht="37.5" spans="1:13">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="13">
+      <c r="K30" s="14">
         <v>7</v>
       </c>
-      <c r="L30" s="15">
+      <c r="L30" s="16">
         <v>51</v>
       </c>
-      <c r="M30" s="5" t="s">
+      <c r="M30" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="K31" s="13">
+      <c r="K31" s="14">
         <v>8</v>
       </c>
-      <c r="L31" s="15">
+      <c r="L31" s="16">
         <v>57</v>
       </c>
-      <c r="M31" s="5" t="s">
+      <c r="M31" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="K32" s="13">
+      <c r="K32" s="14">
         <v>9</v>
       </c>
-      <c r="L32" s="15">
+      <c r="L32" s="16">
         <v>63</v>
       </c>
-      <c r="M32" s="5" t="s">
+      <c r="M32" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="K33" s="16">
+      <c r="K33" s="17">
         <v>10</v>
       </c>
-      <c r="L33" s="17">
+      <c r="L33" s="18">
         <v>69</v>
       </c>
-      <c r="M33" s="18" t="s">
+      <c r="M33" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="6" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3600,27 +3827,28 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B3:J8"/>
+  <dimension ref="B3:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="9.14285714285714" style="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.9047619047619" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.3428571428571" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.0095238095238" style="1" customWidth="1"/>
-    <col min="6" max="7" width="9.14285714285714" style="1"/>
+    <col min="6" max="6" width="13.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.0095238095238" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.6380952380952" style="1" customWidth="1"/>
     <col min="9" max="9" width="12.552380952381" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7619047619048" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:8">
       <c r="B3" s="2" t="s">
         <v>139</v>
       </c>
@@ -3630,36 +3858,36 @@
       <c r="D3" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="H3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J3" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" ht="65.55" customHeight="1" spans="2:9">
-      <c r="B4" s="3" t="s">
+    <row r="4" ht="65.55" customHeight="1" spans="2:7">
+      <c r="B4" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</f>
         <v>=DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I4" s="1" t="str">
+      <c r="G4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_2440730E3B794D249A4BBFB68234E0A5",1)</f>
         <v>=DISPIMG("ID_2440730E3B794D249A4BBFB68234E0A5",1)</v>
       </c>
     </row>
-    <row r="5" ht="37.5" spans="2:9">
+    <row r="5" ht="44" customHeight="1" spans="2:8">
       <c r="B5" s="1" t="s">
         <v>146</v>
       </c>
@@ -3667,58 +3895,108 @@
         <f>_xlfn.DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</f>
         <v>=DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I5" s="1" t="str">
+      <c r="G5" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</f>
         <v>=DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</v>
       </c>
-    </row>
-    <row r="6" ht="39.25" spans="2:9">
-      <c r="B6" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="6" ht="47" customHeight="1" spans="2:7">
+      <c r="B6" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</f>
         <v>=DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="I6" s="1" t="str">
+      <c r="F6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_491D9B3CF8B4441CAD720B86DCA07462",1)</f>
         <v>=DISPIMG("ID_491D9B3CF8B4441CAD720B86DCA07462",1)</v>
       </c>
     </row>
-    <row r="7" ht="59.3" spans="2:4">
+    <row r="7" ht="64" customHeight="1" spans="2:8">
       <c r="B7" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</f>
         <v>=DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" ht="24.3" spans="2:4">
+      <c r="D7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</f>
+        <v>=DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" ht="40" customHeight="1" spans="2:7">
       <c r="B8" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</f>
         <v>=DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>144</v>
+      <c r="D8" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_DD37BC4AF6A646D482F166D1DA3483B9",1)</f>
+        <v>=DISPIMG("ID_DD37BC4AF6A646D482F166D1DA3483B9",1)</v>
+      </c>
+    </row>
+    <row r="9" ht="40" customHeight="1" spans="6:7">
+      <c r="F9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_CC66E0BDF222479FBCA1D73D9EEF98C9",1)</f>
+        <v>=DISPIMG("ID_CC66E0BDF222479FBCA1D73D9EEF98C9",1)</v>
+      </c>
+    </row>
+    <row r="10" ht="33" customHeight="1" spans="6:7">
+      <c r="F10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_69F91952F7254C9081725FDDC3777D6A",1)</f>
+        <v>=DISPIMG("ID_69F91952F7254C9081725FDDC3777D6A",1)</v>
+      </c>
+    </row>
+    <row r="11" ht="50" customHeight="1" spans="6:8">
+      <c r="F11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</f>
+        <v>=DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 6 more missions. Added Pumpling, Magic Candles and Blessed Children as enemies (and boss). Remade Wolf enemy to now move in shape of L, like chess Knight (Horse). Made enemy health bars red and now enemies without mana have no mana bars. Fixed say centering. Added many more trash items as loot. Added gold as loot (now displays as an item you can loot). Added the Fields background. Added Haymaker and Fox Companion spells for Knight and respectively Ranger. Items now display their flavor text and their title centering is fixed.
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23295" windowHeight="13095" activeTab="2"/>
+    <workbookView windowWidth="24225" windowHeight="12495" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
     <sheet name="Monsters" sheetId="2" r:id="rId2"/>
     <sheet name="Traps" sheetId="3" r:id="rId3"/>
+    <sheet name="Spells" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -353,11 +354,86 @@
       </xdr:spPr>
     </xdr:pic>
   </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="ID_B89FB7A8B8234D6EAF929FE5AE44207A" descr="Melee Attack"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3686175" y="2209800"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="ID_D90184E2EFC94DFCB03996685EEFC48E" descr="Charge"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695700" y="3044825"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="ID_797F597F1B7F46D7BFE49889C122C20E" descr="Haymaker"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3790950" y="4854575"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
 </etc:cellImages>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="188">
   <si>
     <t>Player Level</t>
   </si>
@@ -452,13 +528,22 @@
     <t>1 - 2</t>
   </si>
   <si>
-    <t>Town Guard</t>
+    <t>Patrolling Guard</t>
+  </si>
+  <si>
+    <t>Crossbow Guard</t>
+  </si>
+  <si>
+    <t>Shooter</t>
+  </si>
+  <si>
+    <t>Molotov Peasant</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
   <si>
     <t>Serfmaster</t>
-  </si>
-  <si>
-    <t>x2</t>
   </si>
   <si>
     <t>26</t>
@@ -486,6 +571,11 @@
 Lil Munchy has 3 - 4</t>
   </si>
   <si>
+    <t>Marceline is present here
+at the start and tells them
+to kill you or something</t>
+  </si>
+  <si>
     <t>Evil Paprika</t>
   </si>
   <si>
@@ -503,9 +593,6 @@
   </si>
   <si>
     <t>Pumpling</t>
-  </si>
-  <si>
-    <t>0.5</t>
   </si>
   <si>
     <t>10</t>
@@ -584,6 +671,10 @@
 the 2 Guards</t>
   </si>
   <si>
+    <t>He is actually evil and hand
+in hand with Marceline</t>
+  </si>
+  <si>
     <t>Wolf</t>
   </si>
   <si>
@@ -834,6 +925,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Step</t>
     </r>
     <r>
@@ -856,6 +955,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Step</t>
     </r>
     <r>
@@ -883,6 +990,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Death</t>
     </r>
     <r>
@@ -904,6 +1019,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Death</t>
     </r>
     <r>
@@ -930,6 +1053,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Step</t>
     </r>
     <r>
@@ -959,18 +1090,91 @@
     <t>Small chance
 to drop child</t>
   </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Mana Cost</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>100% DMG</t>
+  </si>
+  <si>
+    <t>Fighter</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>2 range
+55% DMG AoE</t>
+  </si>
+  <si>
+    <t>135% DMG</t>
+  </si>
+  <si>
+    <t>Stand Ground</t>
+  </si>
+  <si>
+    <t>Block 90% DMG
+of next Attack;
++1 Damage rest
+of combat</t>
+  </si>
+  <si>
+    <t>Move 1 (free)</t>
+  </si>
+  <si>
+    <t>Haymaker</t>
+  </si>
+  <si>
+    <t>1 range
+75% DMG
+Push 3 away
++ 45% DMG if
+collides</t>
+  </si>
+  <si>
+    <t>Heal 10% HP</t>
+  </si>
+  <si>
+    <t>Indimidation</t>
+  </si>
+  <si>
+    <t>4 range AoE
+Reduces damage
+of enemies by
+25% + 25% of SP
+(doesn't stack)</t>
+  </si>
+  <si>
+    <t>Stun (free)</t>
+  </si>
+  <si>
+    <t>Regeneration</t>
+  </si>
+  <si>
+    <t>Heal 2 + 20% SP
+every turn</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -989,6 +1193,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1033,9 +1245,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1063,27 +1274,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -1105,22 +1295,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1164,7 +1338,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1186,7 +1398,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1204,31 +1416,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1252,7 +1446,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1264,19 +1464,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1294,7 +1488,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1306,25 +1530,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1342,31 +1578,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1610,21 +1822,6 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1670,6 +1867,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1697,15 +1918,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1716,7 +1928,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1734,147 +1946,162 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1883,9 +2110,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1893,6 +2117,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1925,7 +2152,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1988,7 +2215,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2334,565 +2561,565 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="18.7142857142857" style="20" customWidth="1"/>
-    <col min="2" max="2" width="20.4285714285714" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.71428571428571" style="20" customWidth="1"/>
-    <col min="4" max="4" width="11.1428571428571" style="20" customWidth="1"/>
-    <col min="5" max="5" width="13.7142857142857" style="20" customWidth="1"/>
-    <col min="6" max="6" width="17.7142857142857" style="20" customWidth="1"/>
-    <col min="7" max="7" width="17.8571428571429" style="20" customWidth="1"/>
-    <col min="8" max="8" width="17.5714285714286" style="20" customWidth="1"/>
-    <col min="9" max="9" width="19.1428571428571" style="20" customWidth="1"/>
-    <col min="10" max="16384" width="9.14285714285714" style="20"/>
+    <col min="1" max="1" width="18.7142857142857" style="25" customWidth="1"/>
+    <col min="2" max="2" width="20.4285714285714" style="25" customWidth="1"/>
+    <col min="3" max="3" width="9.71428571428571" style="25" customWidth="1"/>
+    <col min="4" max="4" width="11.1428571428571" style="25" customWidth="1"/>
+    <col min="5" max="5" width="13.7142857142857" style="25" customWidth="1"/>
+    <col min="6" max="6" width="17.7142857142857" style="25" customWidth="1"/>
+    <col min="7" max="7" width="17.8571428571429" style="25" customWidth="1"/>
+    <col min="8" max="8" width="17.5714285714286" style="25" customWidth="1"/>
+    <col min="9" max="9" width="19.1428571428571" style="25" customWidth="1"/>
+    <col min="10" max="16384" width="9.14285714285714" style="25"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:9">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="1"/>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="1"/>
-      <c r="B3" s="28">
+      <c r="A3" s="7"/>
+      <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="34">
         <v>20</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="35">
         <v>20</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="36">
         <v>6.5</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="37">
         <v>6.5</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="38">
         <v>6.5</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H3" s="39">
         <v>12</v>
       </c>
-      <c r="I3" s="48">
+      <c r="I3" s="53">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="1"/>
-      <c r="B4" s="28">
+      <c r="A4" s="7"/>
+      <c r="B4" s="33">
         <v>2</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="34">
         <v>21</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="40">
         <v>23</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="34">
         <v>7.5</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="40">
         <v>9</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="7">
         <v>9</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="41">
         <v>15</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="53">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="1"/>
-      <c r="B5" s="28">
+      <c r="A5" s="7"/>
+      <c r="B5" s="33">
         <v>3</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="34">
         <v>22</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="40">
         <v>26</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="36">
         <v>8.5</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="37">
         <v>11.5</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="38">
         <v>11.5</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="41">
         <v>18</v>
       </c>
-      <c r="I5" s="48">
+      <c r="I5" s="53">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="1"/>
-      <c r="B6" s="28">
+      <c r="A6" s="7"/>
+      <c r="B6" s="33">
         <v>4</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="34">
         <v>23</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="40">
         <v>29</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="34">
         <v>9.5</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="40">
         <v>14</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="7">
         <v>14</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="41">
         <v>21</v>
       </c>
-      <c r="I6" s="48">
+      <c r="I6" s="53">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="1"/>
-      <c r="B7" s="28">
+      <c r="A7" s="7"/>
+      <c r="B7" s="33">
         <v>5</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="34">
         <v>24</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="40">
         <v>32</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="36">
         <v>10.5</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="37">
         <v>16.5</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="38">
         <v>16.5</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="41">
         <v>24</v>
       </c>
-      <c r="I7" s="48">
+      <c r="I7" s="53">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="1"/>
-      <c r="B8" s="28">
+      <c r="A8" s="7"/>
+      <c r="B8" s="33">
         <v>6</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="34">
         <v>25</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="40">
         <v>35</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="34">
         <v>11.5</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="40">
         <v>19</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="7">
         <v>19</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="41">
         <v>27</v>
       </c>
-      <c r="I8" s="48">
+      <c r="I8" s="53">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="28">
+      <c r="A9" s="7"/>
+      <c r="B9" s="33">
         <v>7</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="34">
         <v>26</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="40">
         <v>38</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="36">
         <v>12.5</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="37">
         <v>21.5</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="38">
         <v>21.5</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="41">
         <v>30</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="53">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="1"/>
-      <c r="B10" s="28">
+      <c r="A10" s="7"/>
+      <c r="B10" s="33">
         <v>8</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="34">
         <v>27</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="40">
         <v>41</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="34">
         <v>13.5</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="40">
         <v>24</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="7">
         <v>24</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="41">
         <v>33</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="53">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="28">
+      <c r="A11" s="7"/>
+      <c r="B11" s="33">
         <v>9</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="34">
         <v>28</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="40">
         <v>44</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="36">
         <v>14.5</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="37">
         <v>26.5</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="38">
         <v>26.5</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="41">
         <v>36</v>
       </c>
-      <c r="I11" s="48">
+      <c r="I11" s="53">
         <v>50</v>
       </c>
     </row>
     <row r="12" ht="19.5" spans="1:9">
-      <c r="A12" s="1"/>
-      <c r="B12" s="37">
+      <c r="A12" s="7"/>
+      <c r="B12" s="42">
         <v>10</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="43">
         <v>29</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="44">
         <v>47</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="43">
         <v>15.5</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="44">
         <v>29</v>
       </c>
-      <c r="G12" s="40">
+      <c r="G12" s="45">
         <v>29</v>
       </c>
-      <c r="H12" s="41">
+      <c r="H12" s="46">
         <v>39</v>
       </c>
-      <c r="I12" s="49">
+      <c r="I12" s="54">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="1"/>
-      <c r="B16" s="42" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="1"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="1"/>
-      <c r="B17" s="28">
+      <c r="A17" s="7"/>
+      <c r="B17" s="33">
         <v>1</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="39">
         <v>15</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="41">
         <v>1</v>
       </c>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="1"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="1"/>
-      <c r="B18" s="28">
+      <c r="A18" s="7"/>
+      <c r="B18" s="33">
         <v>2</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="41">
         <v>21</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="41">
         <v>1</v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="1"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="1"/>
-      <c r="B19" s="28">
+      <c r="A19" s="7"/>
+      <c r="B19" s="33">
         <v>3</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="41">
         <v>27</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="41">
         <v>2</v>
       </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="1"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="1"/>
-      <c r="B20" s="28">
+      <c r="A20" s="7"/>
+      <c r="B20" s="33">
         <v>4</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="41">
         <v>33</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="36">
+      <c r="E20" s="41">
         <v>2</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="1"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="1"/>
-      <c r="B21" s="28">
+      <c r="A21" s="7"/>
+      <c r="B21" s="33">
         <v>5</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="41">
         <v>39</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="41">
         <v>2</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="1"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="28">
+      <c r="B22" s="33">
         <v>6</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="41">
         <v>45</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="36">
+      <c r="E22" s="41">
         <v>3</v>
       </c>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="28">
+      <c r="B23" s="33">
         <v>7</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="41">
         <v>51</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E23" s="41">
         <v>3</v>
       </c>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="28">
+      <c r="B24" s="33">
         <v>8</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C24" s="41">
         <v>57</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="36">
+      <c r="E24" s="41">
         <v>3</v>
       </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="28">
+      <c r="B25" s="33">
         <v>9</v>
       </c>
-      <c r="C25" s="36">
+      <c r="C25" s="41">
         <v>63</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="36">
+      <c r="E25" s="41">
         <v>4</v>
       </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
     </row>
     <row r="26" spans="2:8">
-      <c r="B26" s="37">
+      <c r="B26" s="42">
         <v>10</v>
       </c>
-      <c r="C26" s="41">
+      <c r="C26" s="46">
         <v>69</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="41">
+      <c r="E26" s="46">
         <v>4</v>
       </c>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30"/>
@@ -2913,175 +3140,175 @@
       <c r="H31"/>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" spans="2:8">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
     </row>
     <row r="35" spans="2:8">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
     </row>
     <row r="36" spans="2:8">
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
     </row>
     <row r="37" spans="2:8">
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
     </row>
     <row r="38" spans="2:8">
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
     </row>
     <row r="39" spans="2:8">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
     </row>
     <row r="40" spans="2:8">
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
     </row>
     <row r="41" spans="2:8">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
     </row>
     <row r="42" spans="2:8">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
     </row>
     <row r="43" spans="2:8">
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
     </row>
     <row r="44" spans="2:8">
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
     </row>
     <row r="45" spans="2:8">
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
     </row>
     <row r="46" spans="2:8">
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
     </row>
     <row r="47" spans="2:8">
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
     </row>
     <row r="48" spans="2:8">
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3092,730 +3319,762 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:N34"/>
+  <dimension ref="A2:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="21.1428571428571" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.5714285714286" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.42857142857143" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.5714285714286" style="6" customWidth="1"/>
-    <col min="5" max="5" width="17.8571428571429" style="6" customWidth="1"/>
-    <col min="6" max="6" width="26" style="6" customWidth="1"/>
-    <col min="7" max="7" width="27" style="6" customWidth="1"/>
-    <col min="8" max="8" width="16.8571428571429" style="6" customWidth="1"/>
-    <col min="9" max="9" width="5" style="6" customWidth="1"/>
-    <col min="10" max="10" width="2.57142857142857" style="6" customWidth="1"/>
-    <col min="11" max="11" width="18.5714285714286" style="6" customWidth="1"/>
-    <col min="12" max="12" width="9.14285714285714" style="6"/>
-    <col min="13" max="13" width="11.5714285714286" style="6" customWidth="1"/>
-    <col min="14" max="14" width="13.4285714285714" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="9.14285714285714" style="6"/>
+    <col min="1" max="1" width="21.1428571428571" style="11" customWidth="1"/>
+    <col min="2" max="2" width="10.5714285714286" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9.42857142857143" style="11" customWidth="1"/>
+    <col min="4" max="4" width="10.5714285714286" style="11" customWidth="1"/>
+    <col min="5" max="5" width="17.8571428571429" style="11" customWidth="1"/>
+    <col min="6" max="6" width="26" style="11" customWidth="1"/>
+    <col min="7" max="7" width="27" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.8571428571429" style="11" customWidth="1"/>
+    <col min="9" max="9" width="36" style="11" customWidth="1"/>
+    <col min="10" max="10" width="2.57142857142857" style="11" customWidth="1"/>
+    <col min="11" max="11" width="18.5714285714286" style="11" customWidth="1"/>
+    <col min="12" max="12" width="9.14285714285714" style="11"/>
+    <col min="13" max="13" width="11.5714285714286" style="11" customWidth="1"/>
+    <col min="14" max="14" width="13.4285714285714" style="11" customWidth="1"/>
+    <col min="15" max="16384" width="9.14285714285714" style="11"/>
   </cols>
   <sheetData>
     <row r="2" spans="14:14">
       <c r="N2"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="15" t="s">
         <v>26</v>
       </c>
       <c r="N3"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="11" t="s">
         <v>30</v>
       </c>
       <c r="N4"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="11">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="11" t="s">
         <v>30</v>
       </c>
       <c r="N5"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="D7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6"/>
-    </row>
-    <row r="7" ht="75" spans="1:14">
-      <c r="A7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="F8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8"/>
+    </row>
+    <row r="9" ht="75" spans="1:14">
+      <c r="A9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9"/>
+    </row>
+    <row r="10" ht="37.5" spans="1:14">
+      <c r="A10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10"/>
+    </row>
+    <row r="11" ht="75" spans="1:14">
+      <c r="A11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13"/>
+    </row>
+    <row r="14" ht="56.25" spans="1:14">
+      <c r="A14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="G14" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="N14"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="N15"/>
+    </row>
+    <row r="16" ht="37.5" spans="1:14">
+      <c r="A16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="11" t="s">
+      <c r="F16" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16"/>
+    </row>
+    <row r="17" ht="56.25" spans="1:14">
+      <c r="A17" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N17"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" ht="56.25" spans="1:6">
+      <c r="A19" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" ht="93.75" spans="1:8">
+      <c r="A20" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="N7"/>
-    </row>
-    <row r="8" ht="37.5" spans="1:14">
-      <c r="A8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N8"/>
-    </row>
-    <row r="9" ht="75" spans="1:14">
-      <c r="A9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="N9"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="C20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" ht="37.5" spans="1:8">
+      <c r="A21" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" ht="37.5" spans="1:8">
+      <c r="A22" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="N11"/>
-    </row>
-    <row r="12" ht="56.25" spans="1:14">
-      <c r="A12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="N12"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="F22" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" ht="37.5" spans="1:7">
+      <c r="A23" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" ht="56.25" spans="1:8">
+      <c r="A24" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" ht="37.5" spans="1:13">
+      <c r="A25" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" ht="56.25" spans="1:13">
+      <c r="A26" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" s="19">
+        <v>1</v>
+      </c>
+      <c r="L26" s="20">
+        <v>15</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" ht="37.5" spans="1:13">
+      <c r="A27" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="K27" s="19">
+        <v>2</v>
+      </c>
+      <c r="L27" s="21">
+        <v>21</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" ht="37.5" spans="1:13">
+      <c r="A28" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="K28" s="19">
+        <v>3</v>
+      </c>
+      <c r="L28" s="21">
+        <v>27</v>
+      </c>
+      <c r="M28" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="N13"/>
-    </row>
-    <row r="14" ht="37.5" spans="1:14">
-      <c r="A14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="N14"/>
-    </row>
-    <row r="15" ht="56.25" spans="1:14">
-      <c r="A15" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="N15"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" ht="56.25" spans="1:6">
-      <c r="A17" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" ht="93.75" spans="1:8">
-      <c r="A18" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" ht="37.5" spans="1:8">
-      <c r="A19" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="6" t="s">
+    </row>
+    <row r="29" ht="56.25" spans="1:13">
+      <c r="A29" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="K29" s="19">
+        <v>4</v>
+      </c>
+      <c r="L29" s="21">
+        <v>33</v>
+      </c>
+      <c r="M29" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" ht="37.5" spans="1:8">
-      <c r="A20" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" ht="37.5" spans="1:7">
-      <c r="A21" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" ht="56.25" spans="1:8">
-      <c r="A22" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" ht="37.5" spans="1:13">
-      <c r="A23" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" ht="56.25" spans="1:13">
-      <c r="A24" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="K24" s="14">
-        <v>1</v>
-      </c>
-      <c r="L24" s="15">
-        <v>15</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" ht="37.5" spans="1:13">
-      <c r="A25" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="K25" s="14">
-        <v>2</v>
-      </c>
-      <c r="L25" s="16">
-        <v>21</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" ht="37.5" spans="1:13">
-      <c r="A26" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="K26" s="14">
-        <v>3</v>
-      </c>
-      <c r="L26" s="16">
-        <v>27</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" ht="56.25" spans="1:13">
-      <c r="A27" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="K27" s="14">
-        <v>4</v>
-      </c>
-      <c r="L27" s="16">
-        <v>33</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" ht="37.5" spans="1:13">
-      <c r="A28" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="K28" s="14">
-        <v>5</v>
-      </c>
-      <c r="L28" s="16">
-        <v>39</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" ht="37.5" spans="1:13">
-      <c r="A29" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="K29" s="14">
-        <v>6</v>
-      </c>
-      <c r="L29" s="16">
-        <v>45</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="30" ht="37.5" spans="1:13">
       <c r="A30" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H30" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K30" s="14">
+      <c r="K30" s="19">
+        <v>5</v>
+      </c>
+      <c r="L30" s="21">
+        <v>39</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" ht="37.5" spans="1:13">
+      <c r="A31" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="K31" s="19">
+        <v>6</v>
+      </c>
+      <c r="L31" s="21">
+        <v>45</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" ht="37.5" spans="1:13">
+      <c r="A32" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" s="19">
         <v>7</v>
       </c>
-      <c r="L30" s="16">
+      <c r="L32" s="21">
         <v>51</v>
       </c>
-      <c r="M30" s="6" t="s">
+      <c r="M32" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="K31" s="14">
+    <row r="33" spans="1:13">
+      <c r="A33" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="K33" s="19">
         <v>8</v>
       </c>
-      <c r="L31" s="16">
+      <c r="L33" s="21">
         <v>57</v>
       </c>
-      <c r="M31" s="6" t="s">
+      <c r="M33" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="K32" s="14">
+    <row r="34" spans="1:13">
+      <c r="A34" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="K34" s="19">
         <v>9</v>
       </c>
-      <c r="L32" s="16">
+      <c r="L34" s="21">
         <v>63</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="M34" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="K33" s="17">
+    <row r="35" spans="1:13">
+      <c r="A35" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="K35" s="22">
         <v>10</v>
       </c>
-      <c r="L33" s="18">
+      <c r="L35" s="23">
         <v>69</v>
       </c>
-      <c r="M33" s="19" t="s">
+      <c r="M35" s="24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>136</v>
+    <row r="36" spans="1:6">
+      <c r="A36" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3829,175 +4088,362 @@
   <sheetPr/>
   <dimension ref="B3:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="1"/>
-    <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.9047619047619" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.3428571428571" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.0095238095238" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.2857142857143" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.0095238095238" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6380952380952" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.552380952381" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.14285714285714" style="1"/>
+    <col min="1" max="1" width="9.14285714285714" style="7"/>
+    <col min="2" max="2" width="16" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.9047619047619" style="7" customWidth="1"/>
+    <col min="4" max="4" width="24.3428571428571" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.0095238095238" style="7" customWidth="1"/>
+    <col min="6" max="6" width="13.2857142857143" style="7" customWidth="1"/>
+    <col min="7" max="7" width="19.0095238095238" style="7" customWidth="1"/>
+    <col min="8" max="8" width="17.6380952380952" style="7" customWidth="1"/>
+    <col min="9" max="9" width="12.552380952381" style="7" customWidth="1"/>
+    <col min="10" max="10" width="19" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="9.14285714285714" style="7"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>141</v>
+      <c r="B3" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="4" ht="65.55" customHeight="1" spans="2:7">
-      <c r="B4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="1" t="str">
+      <c r="B4" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</f>
         <v>=DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G4" s="1" t="str">
+      <c r="D4" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_2440730E3B794D249A4BBFB68234E0A5",1)</f>
         <v>=DISPIMG("ID_2440730E3B794D249A4BBFB68234E0A5",1)</v>
       </c>
     </row>
     <row r="5" ht="44" customHeight="1" spans="2:8">
-      <c r="B5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="1" t="str">
+      <c r="B5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</f>
         <v>=DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" s="1" t="str">
+      <c r="D5" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</f>
         <v>=DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>149</v>
+      <c r="H5" s="9" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" ht="47" customHeight="1" spans="2:7">
-      <c r="B6" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="1" t="str">
+      <c r="B6" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</f>
         <v>=DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G6" s="1" t="str">
+      <c r="D6" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_491D9B3CF8B4441CAD720B86DCA07462",1)</f>
         <v>=DISPIMG("ID_491D9B3CF8B4441CAD720B86DCA07462",1)</v>
       </c>
     </row>
     <row r="7" ht="64" customHeight="1" spans="2:8">
-      <c r="B7" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" s="1" t="str">
+      <c r="B7" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</f>
         <v>=DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G7" s="1" t="str">
+      <c r="D7" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</f>
         <v>=DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>156</v>
+      <c r="H7" s="9" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="8" ht="40" customHeight="1" spans="2:7">
-      <c r="B8" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" s="1" t="str">
+      <c r="B8" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</f>
         <v>=DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G8" s="1" t="str">
+      <c r="D8" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_DD37BC4AF6A646D482F166D1DA3483B9",1)</f>
         <v>=DISPIMG("ID_DD37BC4AF6A646D482F166D1DA3483B9",1)</v>
       </c>
     </row>
     <row r="9" ht="40" customHeight="1" spans="6:7">
-      <c r="F9" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G9" s="1" t="str">
+      <c r="F9" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G9" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_CC66E0BDF222479FBCA1D73D9EEF98C9",1)</f>
         <v>=DISPIMG("ID_CC66E0BDF222479FBCA1D73D9EEF98C9",1)</v>
       </c>
     </row>
     <row r="10" ht="33" customHeight="1" spans="6:7">
-      <c r="F10" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G10" s="1" t="str">
+      <c r="F10" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G10" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_69F91952F7254C9081725FDDC3777D6A",1)</f>
         <v>=DISPIMG("ID_69F91952F7254C9081725FDDC3777D6A",1)</v>
       </c>
     </row>
     <row r="11" ht="50" customHeight="1" spans="6:8">
-      <c r="F11" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G11" s="1" t="str">
+      <c r="F11" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</f>
         <v>=DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>163</v>
-      </c>
+      <c r="H11" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B9:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="9.14285714285714" style="1"/>
+    <col min="2" max="2" width="18.1428571428571" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.7142857142857" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.8571428571429" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.8571428571429" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.5714285714286" style="2" customWidth="1"/>
+    <col min="7" max="9" width="9.14285714285714" style="1"/>
+    <col min="10" max="10" width="18.8571428571429" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.8571428571429" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:11">
+      <c r="B9" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" ht="44" customHeight="1" spans="3:11">
+      <c r="C10" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_B89FB7A8B8234D6EAF929FE5AE44207A",1)</f>
+        <v>=DISPIMG("ID_B89FB7A8B8234D6EAF929FE5AE44207A",1)</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" ht="45" customHeight="1" spans="2:11">
+      <c r="B11" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</f>
+        <v>=DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" ht="75" spans="2:11">
+      <c r="B12" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="97" customHeight="1" spans="2:11">
+      <c r="B13" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</f>
+        <v>=DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="K13" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" ht="93.75" spans="2:11">
+      <c r="B14" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="K14" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" ht="37.5" spans="2:5">
+      <c r="B15" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="7:9">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="7:9">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Crated Highwayman, Reverse Mermaid and Blubber animation. Created the Blubber enemy, which can shoot a splitting bubble. Seems to work fine.
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12495" activeTab="3"/>
+    <workbookView windowWidth="23295" windowHeight="13095" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -429,11 +429,86 @@
       </xdr:spPr>
     </xdr:pic>
   </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="ID_5B5C76B37B874958A231351EBD5A6E7C" descr="Shoot"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3600450" y="7210425"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="ID_52D5A41E637044A490A457D53A6E6968" descr="TripleArrow"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3581400" y="8648700"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="ID_3597ED710A4940C9B87FCDF5F4476A1D" descr="TomeFoxCompanion"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3648075" y="13230225"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
 </etc:cellImages>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="270">
   <si>
     <t>Player Level</t>
   </si>
@@ -1163,6 +1238,320 @@
     <t>Heal 2 + 20% SP
 every turn</t>
   </si>
+  <si>
+    <t>Passive</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
+    <t>Shoot Arrow</t>
+  </si>
+  <si>
+    <t>90% DMG
+4 range</t>
+  </si>
+  <si>
+    <t>Fox Attack</t>
+  </si>
+  <si>
+    <t>35% DMG
+Bleed 35% SP
+global range</t>
+  </si>
+  <si>
+    <t>Quickfoot</t>
+  </si>
+  <si>
+    <t>+1 Movement</t>
+  </si>
+  <si>
+    <t>Triple Arrow</t>
+  </si>
+  <si>
+    <t>85% DMG
+4 range</t>
+  </si>
+  <si>
+    <t>Flareshot</t>
+  </si>
+  <si>
+    <t>90% SP
+4 range (8 way)
+enemy gets -10
+dodge and crit
+(does not stack)</t>
+  </si>
+  <si>
+    <t>105% SP
+4 range (TIR)
+unit gets snared</t>
+  </si>
+  <si>
+    <t>Disorient</t>
+  </si>
+  <si>
+    <t>3 range (TIR)
+Instant
+enemies around
+scatter away from it</t>
+  </si>
+  <si>
+    <t>Steady Shooting</t>
+  </si>
+  <si>
+    <t>Every second shot
+on the same target
+deals 25% extra
+damage</t>
+  </si>
+  <si>
+    <t>Fox Companion</t>
+  </si>
+  <si>
+    <t>Start every combat
+with a Fox companion</t>
+  </si>
+  <si>
+    <t>&lt;Block/Defense&gt;</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Fire Bolt</t>
+  </si>
+  <si>
+    <t>90% SP
+3 range</t>
+  </si>
+  <si>
+    <t>Magic Arrow</t>
+  </si>
+  <si>
+    <t>75% SP + x
+4 range
+diagonally</t>
+  </si>
+  <si>
+    <t>Blink</t>
+  </si>
+  <si>
+    <t>Instant
+Teleport 2 range</t>
+  </si>
+  <si>
+    <t>Mana Ward</t>
+  </si>
+  <si>
+    <t>Any ally
+Shields for
+85% SP + 20% max mana</t>
+  </si>
+  <si>
+    <t>Ice Spike</t>
+  </si>
+  <si>
+    <t>70% SP
+4 range
+Damages all targets
+in a straight line</t>
+  </si>
+  <si>
+    <t>Ignite</t>
+  </si>
+  <si>
+    <t>All enemies bleed</t>
+  </si>
+  <si>
+    <t>Slowdown</t>
+  </si>
+  <si>
+    <t>35% SP
+50% slow
+4 range</t>
+  </si>
+  <si>
+    <t>Conjure Wall</t>
+  </si>
+  <si>
+    <t>4 range
+75% SP health</t>
+  </si>
+  <si>
+    <t>Iceberg Drop</t>
+  </si>
+  <si>
+    <t>40% SP
+4 range (TIR)
+Stuns the target</t>
+  </si>
+  <si>
+    <t>Soul Drain</t>
+  </si>
+  <si>
+    <t>50% SP
+3 range
+If this kills the target,
+gain 1 gem</t>
+  </si>
+  <si>
+    <t>&lt;Buff&gt;</t>
+  </si>
+  <si>
+    <t>Rogue</t>
+  </si>
+  <si>
+    <t>Flank</t>
+  </si>
+  <si>
+    <t>110% DMG
+diagonally</t>
+  </si>
+  <si>
+    <t>Backstab</t>
+  </si>
+  <si>
+    <t>135% DMG + x
+left only</t>
+  </si>
+  <si>
+    <t>Shadowstep</t>
+  </si>
+  <si>
+    <t>Teleport 3 range
+Instant
+Next attack ignores armor
+(TIR)</t>
+  </si>
+  <si>
+    <t>Pocket Sand</t>
+  </si>
+  <si>
+    <t>2 range
+8 way
+Stuns the target
+and pushes it
+random direction</t>
+  </si>
+  <si>
+    <t>Hijack</t>
+  </si>
+  <si>
+    <t>Rob Them Blind</t>
+  </si>
+  <si>
+    <t>Instant
+Increases gold loot
+gained by 25%
+(stacks)</t>
+  </si>
+  <si>
+    <t>&lt;Debuff&gt;</t>
+  </si>
+  <si>
+    <t>Fighter
+Ranger
+Rogue</t>
+  </si>
+  <si>
+    <t>Bandage</t>
+  </si>
+  <si>
+    <t>Heal 75% SP
+1 range, 8 way</t>
+  </si>
+  <si>
+    <t>Fighter, Rogue</t>
+  </si>
+  <si>
+    <t>Whirlwind</t>
+  </si>
+  <si>
+    <t>70% DMG
+ AoE
+1 range, 8 way</t>
+  </si>
+  <si>
+    <t>Fighter, Mage</t>
+  </si>
+  <si>
+    <t>Thunderclap</t>
+  </si>
+  <si>
+    <t>60% SP
+3 range, AoE</t>
+  </si>
+  <si>
+    <t>Figher, Ranger</t>
+  </si>
+  <si>
+    <t>Raise Morale</t>
+  </si>
+  <si>
+    <t>All allies +15% DMG
+and +2 initiative
+(does not stack)
+Instant</t>
+  </si>
+  <si>
+    <t>Thrown Skiver</t>
+  </si>
+  <si>
+    <t>15% DMG + bleed
+3 range, but jump
+over the first tile</t>
+  </si>
+  <si>
+    <t>Fighter
+Mage
+Rogue</t>
+  </si>
+  <si>
+    <t>Blood Drain</t>
+  </si>
+  <si>
+    <t>65% SP damage
+Heal 40% SP
+2 range, diagonal</t>
+  </si>
+  <si>
+    <t>Ranger, Rogue</t>
+  </si>
+  <si>
+    <t>Fence</t>
+  </si>
+  <si>
+    <t>Gain 50% dodge
+2 turns
+Instant</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Vampirism</t>
+  </si>
+  <si>
+    <t>Heal for 15% of
+damage dealt</t>
+  </si>
+  <si>
+    <t>Figher
+Ranger
+Rogue</t>
+  </si>
+  <si>
+    <t>Magic Touch</t>
+  </si>
+  <si>
+    <t>Your normal attacks
+or arrows deal
++25% SP damage</t>
+  </si>
 </sst>
 </file>
 
@@ -1170,11 +1559,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1201,6 +1590,20 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4" tint="-0.25"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1246,6 +1649,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1253,14 +1663,47 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1269,6 +1712,20 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1284,7 +1741,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1299,7 +1771,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1313,77 +1785,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1398,31 +1801,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1434,85 +1843,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1530,7 +1861,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1542,37 +1963,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1826,54 +2229,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1885,17 +2240,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1917,9 +2261,68 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1928,7 +2331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1946,134 +2349,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2083,9 +2486,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2095,33 +2495,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2149,10 +2552,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2215,7 +2615,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2237,6 +2637,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2566,560 +2969,560 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="18.7142857142857" style="25" customWidth="1"/>
-    <col min="2" max="2" width="20.4285714285714" style="25" customWidth="1"/>
-    <col min="3" max="3" width="9.71428571428571" style="25" customWidth="1"/>
-    <col min="4" max="4" width="11.1428571428571" style="25" customWidth="1"/>
-    <col min="5" max="5" width="13.7142857142857" style="25" customWidth="1"/>
-    <col min="6" max="6" width="17.7142857142857" style="25" customWidth="1"/>
-    <col min="7" max="7" width="17.8571428571429" style="25" customWidth="1"/>
-    <col min="8" max="8" width="17.5714285714286" style="25" customWidth="1"/>
-    <col min="9" max="9" width="19.1428571428571" style="25" customWidth="1"/>
-    <col min="10" max="16384" width="9.14285714285714" style="25"/>
+    <col min="1" max="1" width="18.7142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.4285714285714" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.71428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1428571428571" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7142857142857" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.8571428571429" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5714285714286" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1428571428571" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:9">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="7"/>
-      <c r="B2" s="26" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="7"/>
-      <c r="B3" s="33">
+      <c r="A3" s="2"/>
+      <c r="B3" s="32">
         <v>1</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="33">
         <v>20</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="34">
         <v>20</v>
       </c>
-      <c r="E3" s="36">
+      <c r="E3" s="35">
         <v>6.5</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="36">
         <v>6.5</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="37">
         <v>6.5</v>
       </c>
-      <c r="H3" s="39">
+      <c r="H3" s="38">
         <v>12</v>
       </c>
-      <c r="I3" s="53">
+      <c r="I3" s="52">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="7"/>
-      <c r="B4" s="33">
+      <c r="A4" s="2"/>
+      <c r="B4" s="32">
         <v>2</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="33">
         <v>21</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="39">
         <v>23</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="33">
         <v>7.5</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="39">
         <v>9</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="2">
         <v>9</v>
       </c>
-      <c r="H4" s="41">
+      <c r="H4" s="40">
         <v>15</v>
       </c>
-      <c r="I4" s="53">
+      <c r="I4" s="52">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="7"/>
-      <c r="B5" s="33">
+      <c r="A5" s="2"/>
+      <c r="B5" s="32">
         <v>3</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="33">
         <v>22</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="39">
         <v>26</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="35">
         <v>8.5</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="36">
         <v>11.5</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="37">
         <v>11.5</v>
       </c>
-      <c r="H5" s="41">
+      <c r="H5" s="40">
         <v>18</v>
       </c>
-      <c r="I5" s="53">
+      <c r="I5" s="52">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="7"/>
-      <c r="B6" s="33">
+      <c r="A6" s="2"/>
+      <c r="B6" s="32">
         <v>4</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="33">
         <v>23</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="39">
         <v>29</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="33">
         <v>9.5</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="39">
         <v>14</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="2">
         <v>14</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H6" s="40">
         <v>21</v>
       </c>
-      <c r="I6" s="53">
+      <c r="I6" s="52">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="7"/>
-      <c r="B7" s="33">
+      <c r="A7" s="2"/>
+      <c r="B7" s="32">
         <v>5</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="33">
         <v>24</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="39">
         <v>32</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="35">
         <v>10.5</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="36">
         <v>16.5</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="37">
         <v>16.5</v>
       </c>
-      <c r="H7" s="41">
+      <c r="H7" s="40">
         <v>24</v>
       </c>
-      <c r="I7" s="53">
+      <c r="I7" s="52">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="7"/>
-      <c r="B8" s="33">
+      <c r="A8" s="2"/>
+      <c r="B8" s="32">
         <v>6</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="33">
         <v>25</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="39">
         <v>35</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="33">
         <v>11.5</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="39">
         <v>19</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="2">
         <v>19</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H8" s="40">
         <v>27</v>
       </c>
-      <c r="I8" s="53">
+      <c r="I8" s="52">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="7"/>
-      <c r="B9" s="33">
+      <c r="A9" s="2"/>
+      <c r="B9" s="32">
         <v>7</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="33">
         <v>26</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="39">
         <v>38</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="35">
         <v>12.5</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="36">
         <v>21.5</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="37">
         <v>21.5</v>
       </c>
-      <c r="H9" s="41">
+      <c r="H9" s="40">
         <v>30</v>
       </c>
-      <c r="I9" s="53">
+      <c r="I9" s="52">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="7"/>
-      <c r="B10" s="33">
+      <c r="A10" s="2"/>
+      <c r="B10" s="32">
         <v>8</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="33">
         <v>27</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="39">
         <v>41</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="33">
         <v>13.5</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="39">
         <v>24</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="2">
         <v>24</v>
       </c>
-      <c r="H10" s="41">
+      <c r="H10" s="40">
         <v>33</v>
       </c>
-      <c r="I10" s="53">
+      <c r="I10" s="52">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="7"/>
-      <c r="B11" s="33">
+      <c r="A11" s="2"/>
+      <c r="B11" s="32">
         <v>9</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="33">
         <v>28</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="39">
         <v>44</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="35">
         <v>14.5</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="36">
         <v>26.5</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="37">
         <v>26.5</v>
       </c>
-      <c r="H11" s="41">
+      <c r="H11" s="40">
         <v>36</v>
       </c>
-      <c r="I11" s="53">
+      <c r="I11" s="52">
         <v>50</v>
       </c>
     </row>
     <row r="12" ht="19.5" spans="1:9">
-      <c r="A12" s="7"/>
-      <c r="B12" s="42">
+      <c r="A12" s="2"/>
+      <c r="B12" s="41">
         <v>10</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="42">
         <v>29</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="43">
         <v>47</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="42">
         <v>15.5</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="43">
         <v>29</v>
       </c>
-      <c r="G12" s="45">
+      <c r="G12" s="44">
         <v>29</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>39</v>
       </c>
-      <c r="I12" s="54">
+      <c r="I12" s="53">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="7"/>
-      <c r="B16" s="47" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="7"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="7"/>
-      <c r="B17" s="33">
+      <c r="A17" s="2"/>
+      <c r="B17" s="32">
         <v>1</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="38">
         <v>15</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="41">
+      <c r="E17" s="40">
         <v>1</v>
       </c>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="7"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="7"/>
-      <c r="B18" s="33">
+      <c r="A18" s="2"/>
+      <c r="B18" s="32">
         <v>2</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="40">
         <v>21</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="40">
         <v>1</v>
       </c>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="7"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="7"/>
-      <c r="B19" s="33">
+      <c r="A19" s="2"/>
+      <c r="B19" s="32">
         <v>3</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="40">
         <v>27</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="41">
+      <c r="E19" s="40">
         <v>2</v>
       </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="7"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="7"/>
-      <c r="B20" s="33">
+      <c r="A20" s="2"/>
+      <c r="B20" s="32">
         <v>4</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="40">
         <v>33</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="41">
+      <c r="E20" s="40">
         <v>2</v>
       </c>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="7"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="7"/>
-      <c r="B21" s="33">
+      <c r="A21" s="2"/>
+      <c r="B21" s="32">
         <v>5</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="40">
         <v>39</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="40">
         <v>2</v>
       </c>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="7"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="33">
+      <c r="B22" s="32">
         <v>6</v>
       </c>
-      <c r="C22" s="41">
+      <c r="C22" s="40">
         <v>45</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="41">
+      <c r="E22" s="40">
         <v>3</v>
       </c>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="33">
+      <c r="B23" s="32">
         <v>7</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="40">
         <v>51</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="41">
+      <c r="E23" s="40">
         <v>3</v>
       </c>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="33">
+      <c r="B24" s="32">
         <v>8</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="40">
         <v>57</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="40">
         <v>3</v>
       </c>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="33">
+      <c r="B25" s="32">
         <v>9</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="40">
         <v>63</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="41">
+      <c r="E25" s="40">
         <v>4</v>
       </c>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
     </row>
     <row r="26" spans="2:8">
-      <c r="B26" s="42">
+      <c r="B26" s="41">
         <v>10</v>
       </c>
-      <c r="C26" s="46">
+      <c r="C26" s="45">
         <v>69</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="46">
+      <c r="E26" s="45">
         <v>4</v>
       </c>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
     </row>
     <row r="30" spans="2:8">
       <c r="B30"/>
@@ -3348,10 +3751,10 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -3438,7 +3841,6 @@
       <c r="A8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
         <v>28</v>
       </c>
@@ -3502,7 +3904,6 @@
       <c r="A11" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="11"/>
       <c r="C11" s="11" t="s">
         <v>46</v>
       </c>
@@ -4094,167 +4495,167 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="7"/>
-    <col min="2" max="2" width="16" style="7" customWidth="1"/>
-    <col min="3" max="3" width="14.9047619047619" style="7" customWidth="1"/>
-    <col min="4" max="4" width="24.3428571428571" style="7" customWidth="1"/>
-    <col min="5" max="5" width="17.0095238095238" style="7" customWidth="1"/>
-    <col min="6" max="6" width="13.2857142857143" style="7" customWidth="1"/>
-    <col min="7" max="7" width="19.0095238095238" style="7" customWidth="1"/>
-    <col min="8" max="8" width="17.6380952380952" style="7" customWidth="1"/>
-    <col min="9" max="9" width="12.552380952381" style="7" customWidth="1"/>
-    <col min="10" max="10" width="19" style="7" customWidth="1"/>
-    <col min="11" max="16384" width="9.14285714285714" style="7"/>
+    <col min="1" max="1" width="9.14285714285714" style="2"/>
+    <col min="2" max="2" width="16" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.9047619047619" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.3428571428571" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.0095238095238" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.2857142857143" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.0095238095238" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.6380952380952" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.552380952381" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.14285714285714" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="4" ht="65.55" customHeight="1" spans="2:7">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="7" t="str">
+      <c r="C4" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</f>
         <v>=DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="7" t="str">
+      <c r="G4" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_2440730E3B794D249A4BBFB68234E0A5",1)</f>
         <v>=DISPIMG("ID_2440730E3B794D249A4BBFB68234E0A5",1)</v>
       </c>
     </row>
     <row r="5" ht="44" customHeight="1" spans="2:8">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="7" t="str">
+      <c r="C5" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</f>
         <v>=DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="7" t="str">
+      <c r="G5" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</f>
         <v>=DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="6" ht="47" customHeight="1" spans="2:7">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="7" t="str">
+      <c r="C6" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</f>
         <v>=DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G6" s="7" t="str">
+      <c r="G6" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_491D9B3CF8B4441CAD720B86DCA07462",1)</f>
         <v>=DISPIMG("ID_491D9B3CF8B4441CAD720B86DCA07462",1)</v>
       </c>
     </row>
     <row r="7" ht="64" customHeight="1" spans="2:8">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="7" t="str">
+      <c r="C7" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</f>
         <v>=DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G7" s="7" t="str">
+      <c r="G7" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</f>
         <v>=DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="10" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="8" ht="40" customHeight="1" spans="2:7">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C8" s="7" t="str">
+      <c r="C8" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</f>
         <v>=DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G8" s="7" t="str">
+      <c r="G8" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_DD37BC4AF6A646D482F166D1DA3483B9",1)</f>
         <v>=DISPIMG("ID_DD37BC4AF6A646D482F166D1DA3483B9",1)</v>
       </c>
     </row>
     <row r="9" ht="40" customHeight="1" spans="6:7">
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G9" s="7" t="str">
+      <c r="G9" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_CC66E0BDF222479FBCA1D73D9EEF98C9",1)</f>
         <v>=DISPIMG("ID_CC66E0BDF222479FBCA1D73D9EEF98C9",1)</v>
       </c>
     </row>
     <row r="10" ht="33" customHeight="1" spans="6:7">
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G10" s="7" t="str">
+      <c r="G10" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_69F91952F7254C9081725FDDC3777D6A",1)</f>
         <v>=DISPIMG("ID_69F91952F7254C9081725FDDC3777D6A",1)</v>
       </c>
     </row>
     <row r="11" ht="50" customHeight="1" spans="6:8">
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G11" s="7" t="str">
+      <c r="G11" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</f>
         <v>=DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="10" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4267,10 +4668,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B9:K23"/>
+  <dimension ref="B9:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4282,31 +4683,31 @@
     <col min="5" max="5" width="21.8571428571429" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.5714285714286" style="2" customWidth="1"/>
     <col min="7" max="9" width="9.14285714285714" style="1"/>
-    <col min="10" max="10" width="18.8571428571429" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.8571428571429" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.8571428571429" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.8571428571429" style="2" customWidth="1"/>
     <col min="12" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="2:11">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4324,10 +4725,10 @@
       <c r="F10" s="2">
         <v>0</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4342,16 +4743,16 @@
         <f>_xlfn.DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</f>
         <v>=DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>175</v>
       </c>
       <c r="F11" s="2">
         <v>2</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="2">
         <v>2</v>
       </c>
     </row>
@@ -4362,16 +4763,16 @@
       <c r="C12" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>178</v>
       </c>
       <c r="F12" s="2">
         <v>4</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="2">
         <v>1</v>
       </c>
     </row>
@@ -4386,16 +4787,16 @@
         <f>_xlfn.DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</f>
         <v>=DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>181</v>
       </c>
       <c r="F13" s="2">
         <v>3</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="2">
         <v>5</v>
       </c>
     </row>
@@ -4406,44 +4807,596 @@
       <c r="C14" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>184</v>
       </c>
       <c r="F14" s="2">
         <v>5</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="15" ht="37.5" spans="2:5">
+    <row r="15" ht="37.5" spans="2:6">
       <c r="B15" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="21" spans="7:9">
+      <c r="F15" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" ht="37.5" spans="2:6">
+      <c r="B16" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_5B5C76B37B874958A231351EBD5A6E7C",1)</f>
+        <v>=DISPIMG("ID_5B5C76B37B874958A231351EBD5A6E7C",1)</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" ht="56.25" spans="2:6">
+      <c r="B17" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" ht="37.5" spans="2:6">
+      <c r="B19" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_52D5A41E637044A490A457D53A6E6968",1)</f>
+        <v>=DISPIMG("ID_52D5A41E637044A490A457D53A6E6968",1)</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" ht="93.75" spans="2:6">
+      <c r="B20" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" ht="56.25" spans="2:9">
+      <c r="B21" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="7:9">
+    <row r="22" ht="93.75" spans="2:9">
+      <c r="B22" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F22" s="2">
+        <v>3</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="7:9">
+    <row r="23" ht="75" spans="2:9">
+      <c r="B23" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
+    </row>
+    <row r="24" ht="56.25" spans="2:6">
+      <c r="B24" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_3597ED710A4940C9B87FCDF5F4476A1D",1)</f>
+        <v>=DISPIMG("ID_3597ED710A4940C9B87FCDF5F4476A1D",1)</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" ht="37.5" spans="2:6">
+      <c r="B26" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" ht="56.25" spans="2:6">
+      <c r="B27" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" ht="37.5" spans="2:6">
+      <c r="B28" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F28" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" ht="75" spans="2:6">
+      <c r="B29" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F29" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" ht="93.75" spans="2:6">
+      <c r="B30" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F31" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" ht="56.25" spans="2:6">
+      <c r="B32" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" ht="37.5" spans="2:6">
+      <c r="B33" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F33" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" ht="56.25" spans="2:6">
+      <c r="B34" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F34" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" ht="93.75" spans="2:5">
+      <c r="B35" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" ht="37.5" spans="2:6">
+      <c r="B38" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F38" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" ht="37.5" spans="2:6">
+      <c r="B39" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F39" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" ht="93.75" spans="2:6">
+      <c r="B40" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F40" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" ht="93.75" spans="2:6">
+      <c r="B41" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F41" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="43" ht="75" spans="2:6">
+      <c r="B43" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F43" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" ht="56.25" spans="2:6">
+      <c r="B46" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F46" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" ht="56.25" spans="2:6">
+      <c r="B47" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F47" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" ht="37.5" spans="2:6">
+      <c r="B48" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F48" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" ht="93.75" spans="2:6">
+      <c r="B49" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F49" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" ht="56.25" spans="2:6">
+      <c r="B50" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F50" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" ht="56.25" spans="2:6">
+      <c r="B51" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F51" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" ht="56.25" spans="2:6">
+      <c r="B52" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F52" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" ht="37.5" spans="2:6">
+      <c r="B53" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="54" ht="75" spans="2:6">
+      <c r="B54" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>188</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added many spells (working): Bear Trap, Disorient, Flare Shot, Fox Attack, Intimidation, Stand Ground, Quickfoot and Regeneration. Implemented buff system. Simple and working very well!
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23295" windowHeight="13095" activeTab="3"/>
+    <workbookView windowWidth="20025" windowHeight="12345" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -504,6 +504,206 @@
       </xdr:spPr>
     </xdr:pic>
   </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="ID_3B6DDDD98A8F40BC81817AB7D481E31C" descr="Flare Shot"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3724275" y="9582150"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="ID_9DEEB880DCB04491A4378D1013CB4998" descr="Bear Trap"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3752850" y="10582275"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="ID_937E3FF1032A441DAFCEF81E0E8651CE" descr="Disorient"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3590925" y="11515725"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="ID_601DEB5433E749A5B04D3AB579BF0284" descr="Stand Ground"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3762375" y="3883025"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="ID_900DEDBC95DA49B6832F8E0EAF3922E7" descr="Intimidation"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695700" y="6105525"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="ID_05B2EF6AB8B64DED9EE5B9B0C23F991B" descr="TomeQuickfoot"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3819525" y="8553450"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="ID_6D29D48731D64D15B7AFC6A55F3580E6" descr="TomeRegeneration"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3762375" y="7067550"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="ID_B7F3E8AB96A746EEA8D18747E89057C6" descr="Fox Attack"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3781425" y="8334375"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
 </etc:cellImages>
 </file>
 
@@ -1197,8 +1397,8 @@
     <t>Stand Ground</t>
   </si>
   <si>
-    <t>Block 90% DMG
-of next Attack;
+    <t>Block 60% DMG
+until next turn;
 +1 Damage rest
 of combat</t>
   </si>
@@ -1222,10 +1422,10 @@
     <t>Indimidation</t>
   </si>
   <si>
-    <t>4 range AoE
+    <t>5 range AoE
 Reduces damage
 of enemies by
-25% + 25% of SP
+25% + damages 30% of SP
 (doesn't stack)</t>
   </si>
   <si>
@@ -1235,7 +1435,7 @@
     <t>Regeneration</t>
   </si>
   <si>
-    <t>Heal 2 + 20% SP
+    <t>Heal 1 + 20% SP
 every turn</t>
   </si>
   <si>
@@ -1257,7 +1457,8 @@
   <si>
     <t>35% DMG
 Bleed 35% SP
-global range</t>
+global range
+(3 turns)</t>
   </si>
   <si>
     <t>Quickfoot</t>
@@ -1273,7 +1474,7 @@
 4 range</t>
   </si>
   <si>
-    <t>Flareshot</t>
+    <t>Flare Shot</t>
   </si>
   <si>
     <t>90% SP
@@ -1285,7 +1486,7 @@
   <si>
     <t>105% SP
 4 range (TIR)
-unit gets snared</t>
+(instant)</t>
   </si>
   <si>
     <t>Disorient</t>
@@ -1558,10 +1759,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1649,21 +1850,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1671,7 +1865,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1685,25 +1879,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1718,14 +1895,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1736,6 +1914,45 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1754,39 +1971,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1801,37 +2002,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1843,31 +2020,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1885,7 +2044,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1897,19 +2128,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1921,7 +2140,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1939,25 +2170,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1969,19 +2182,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2244,50 +2445,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2313,6 +2470,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -2326,12 +2507,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2349,130 +2550,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2964,7 +3165,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -3725,7 +3926,7 @@
   <dimension ref="A2:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4490,7 +4691,7 @@
   <dimension ref="B3:H11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="7"/>
@@ -4670,8 +4871,8 @@
   <sheetPr/>
   <dimension ref="B9:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4763,6 +4964,10 @@
       <c r="C12" s="2" t="s">
         <v>177</v>
       </c>
+      <c r="D12" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_601DEB5433E749A5B04D3AB579BF0284",1)</f>
+        <v>=DISPIMG("ID_601DEB5433E749A5B04D3AB579BF0284",1)</v>
+      </c>
       <c r="E12" s="5" t="s">
         <v>178</v>
       </c>
@@ -4800,12 +5005,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" ht="93.75" spans="2:11">
+    <row r="14" ht="112.5" spans="2:11">
       <c r="B14" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>183</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_900DEDBC95DA49B6832F8E0EAF3922E7",1)</f>
+        <v>=DISPIMG("ID_900DEDBC95DA49B6832F8E0EAF3922E7",1)</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>184</v>
@@ -4827,6 +5036,10 @@
       <c r="C15" s="6" t="s">
         <v>186</v>
       </c>
+      <c r="D15" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</f>
+        <v>=DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</v>
+      </c>
       <c r="E15" s="5" t="s">
         <v>187</v>
       </c>
@@ -4852,26 +5065,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" ht="56.25" spans="2:6">
+    <row r="17" ht="75" spans="2:6">
       <c r="B17" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>192</v>
       </c>
+      <c r="D17" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_B7F3E8AB96A746EEA8D18747E89057C6",1)</f>
+        <v>=DISPIMG("ID_B7F3E8AB96A746EEA8D18747E89057C6",1)</v>
+      </c>
       <c r="E17" s="5" t="s">
         <v>193</v>
       </c>
       <c r="F17" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" ht="29.25" spans="2:6">
       <c r="B18" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>194</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_05B2EF6AB8B64DED9EE5B9B0C23F991B",1)</f>
+        <v>=DISPIMG("ID_05B2EF6AB8B64DED9EE5B9B0C23F991B",1)</v>
       </c>
       <c r="E18" s="54" t="s">
         <v>195</v>
@@ -4905,6 +5126,10 @@
       <c r="C20" s="2" t="s">
         <v>198</v>
       </c>
+      <c r="D20" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_3B6DDDD98A8F40BC81817AB7D481E31C",1)</f>
+        <v>=DISPIMG("ID_3B6DDDD98A8F40BC81817AB7D481E31C",1)</v>
+      </c>
       <c r="E20" s="5" t="s">
         <v>199</v>
       </c>
@@ -4919,6 +5144,10 @@
       <c r="C21" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="D21" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_9DEEB880DCB04491A4378D1013CB4998",1)</f>
+        <v>=DISPIMG("ID_9DEEB880DCB04491A4378D1013CB4998",1)</v>
+      </c>
       <c r="E21" s="7" t="s">
         <v>200</v>
       </c>
@@ -4935,6 +5164,10 @@
       </c>
       <c r="C22" s="2" t="s">
         <v>201</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f>_xlfn.DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</f>
+        <v>=DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>202</v>

</xml_diff>

<commit_message>
Shooter AI now moves the shooter away from player units if its near. Fixed pathing issues for large units. Made cave background. Shopkeepers say something when you buy something.
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23295" windowHeight="13095" activeTab="1"/>
+    <workbookView windowWidth="24225" windowHeight="12495" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -933,11 +933,167 @@
       </xdr:spPr>
     </xdr:pic>
   </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="ID_163A9240D4EF485292D7AE5FEFA9852F" descr="highwayman"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId37"/>
+        <a:srcRect r="84722"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1638300" y="8206105"/>
+          <a:ext cx="990600" cy="1080770"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="ID_7ED09DD668894ABE8A725CF2D4D0029F" descr="guard"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId38"/>
+        <a:srcRect r="83854"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1695450" y="9280525"/>
+          <a:ext cx="885825" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="ID_D36F8EAEDC3D4A2D9DDF24AE96ABB005" descr="Rat"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId39"/>
+        <a:srcRect t="30208" r="78750"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1714500" y="10290175"/>
+          <a:ext cx="971550" cy="638175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="ID_A046AFD9A3BF492EADA57F8350871DB2" descr="Peasant3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId40"/>
+        <a:srcRect t="25000" r="83160"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1558290" y="11109960"/>
+          <a:ext cx="1089660" cy="808990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="ID_2AC053A6DE184E4097DCE1BD0082E519" descr="WolfAnimated"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId41"/>
+        <a:srcRect r="79874"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1504950" y="12033250"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="ID_D72C5AF664FF4D6C8BB8BF8BE922256D" descr="Bubak"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId42"/>
+        <a:srcRect t="2083" r="73958"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1895475" y="13658850"/>
+          <a:ext cx="952500" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
 </etc:cellImages>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="334">
   <si>
     <t>Player Level</t>
   </si>
@@ -1068,7 +1224,7 @@
     <t>Targets a random tile
 in range.
 Leaves fire on the
-ground there + 1 adjacent</t>
+ground there</t>
   </si>
   <si>
     <t>Killable in 1 + 2 shot</t>
@@ -1077,12 +1233,15 @@
     <t>Serfmaster</t>
   </si>
   <si>
-    <t>26</t>
+    <t>22</t>
   </si>
   <si>
     <t>Large</t>
   </si>
   <si>
+    <t>Attacks push 1</t>
+  </si>
+  <si>
     <t>Has 6*4 + 2 HP</t>
   </si>
   <si>
@@ -1108,6 +1267,12 @@
   </si>
   <si>
     <t>Can't heal self</t>
+  </si>
+  <si>
+    <t>Pumpling</t>
+  </si>
+  <si>
+    <t>50% dodge chance</t>
   </si>
   <si>
     <t>Evil Paprika</t>
@@ -1126,10 +1291,74 @@
 (delayed)</t>
   </si>
   <si>
-    <t>Pumpling</t>
-  </si>
-  <si>
-    <t>50% dodge chance</t>
+    <t>Highwayman</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Marks a cluster of
+3 tiles.
+Shoots them next turn</t>
+  </si>
+  <si>
+    <t>Guard</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>Whenever a player
+moves, gain 1 Armor</t>
+  </si>
+  <si>
+    <t>Attacks pierce
+and reach 2</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Attacks diagonally</t>
+  </si>
+  <si>
+    <t>Whenever an ally dies,
+gain 1 attack</t>
+  </si>
+  <si>
+    <t>Immune to Acid</t>
+  </si>
+  <si>
+    <t>Bandit Peasant</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>Moves in shape of L</t>
+  </si>
+  <si>
+    <t>Bubak</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Heals allies around
+for 5 hp every turn
+and shreds all block</t>
+  </si>
+  <si>
+    <t>When it dies, all allies:
++10% crit
++10% dodge
++1 magic resistance</t>
   </si>
   <si>
     <t>THE PAGAN TRIO</t>
@@ -1165,12 +1394,6 @@
     <t>Heavenly Spirit</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>Fly</t>
   </si>
   <si>
@@ -1197,9 +1420,6 @@
   <si>
     <t>He is actually evil and hand
 in hand with Marceline</t>
-  </si>
-  <si>
-    <t>Wolf</t>
   </si>
   <si>
     <t>25</t>
@@ -1214,9 +1434,6 @@
 beta wolf</t>
   </si>
   <si>
-    <t>Highwayman</t>
-  </si>
-  <si>
     <t>24</t>
   </si>
   <si>
@@ -1291,9 +1508,6 @@
   </si>
   <si>
     <t>Slime</t>
-  </si>
-  <si>
-    <t>22</t>
   </si>
   <si>
     <t>Splits into 2 smaller
@@ -1723,14 +1937,21 @@
     <t>Stun (free)</t>
   </si>
   <si>
+    <t>Kill Block</t>
+  </si>
+  <si>
+    <t>After killing a unit,
+cast Block</t>
+  </si>
+  <si>
+    <t>Passive</t>
+  </si>
+  <si>
     <t>Regeneration</t>
   </si>
   <si>
     <t>Heal 1 + 20% SP
 every turn</t>
-  </si>
-  <si>
-    <t>Passive</t>
   </si>
   <si>
     <t>Ranger</t>
@@ -2215,10 +2436,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -2313,19 +2534,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2336,9 +2565,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2351,17 +2579,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2376,9 +2612,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2390,23 +2634,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2420,9 +2649,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2435,23 +2670,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2466,13 +2687,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2484,7 +2765,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2502,151 +2855,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2964,39 +3185,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -3027,6 +3215,48 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3038,15 +3268,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3066,15 +3287,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -3084,130 +3305,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3738,7 +3959,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4463,12 +4684,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4479,7 +4700,7 @@
     <col min="5" max="5" width="17.8571428571429" style="22" customWidth="1"/>
     <col min="6" max="6" width="26" style="22" customWidth="1"/>
     <col min="7" max="7" width="27" style="22" customWidth="1"/>
-    <col min="8" max="8" width="16.8571428571429" style="22" customWidth="1"/>
+    <col min="8" max="8" width="23.7142857142857" style="22" customWidth="1"/>
     <col min="9" max="9" width="36" style="22" customWidth="1"/>
     <col min="10" max="10" width="2.57142857142857" style="22" customWidth="1"/>
     <col min="11" max="11" width="18.5714285714286" style="22" customWidth="1"/>
@@ -4587,7 +4808,7 @@
       </c>
       <c r="N4"/>
     </row>
-    <row r="5" ht="58" customHeight="1" spans="1:14">
+    <row r="5" ht="87" customHeight="1" spans="1:14">
       <c r="A5" s="22" t="s">
         <v>39</v>
       </c>
@@ -4632,14 +4853,17 @@
       <c r="F6" s="22" t="s">
         <v>46</v>
       </c>
+      <c r="G6" s="22" t="s">
+        <v>47</v>
+      </c>
       <c r="I6" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N6"/>
     </row>
     <row r="7" ht="58" customHeight="1" spans="1:14">
       <c r="A7" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" s="27" t="str">
         <f>_xlfn.DISPIMG("ID_5DCB40CCA6B44244B7519B2BA06EDF1C",1)</f>
@@ -4652,16 +4876,16 @@
         <v>29</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N7"/>
     </row>
     <row r="8" ht="71" customHeight="1" spans="1:14">
       <c r="A8" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8" s="30" t="str">
         <f>_xlfn.DISPIMG("ID_9997CD209D774EEAB420C53DDEA056A0",1)</f>
@@ -4671,601 +4895,756 @@
         <v>29</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N8"/>
     </row>
-    <row r="9" ht="71" customHeight="1" spans="1:14">
+    <row r="9" ht="75" customHeight="1" spans="1:14">
       <c r="A9" s="22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" s="27" t="str">
+        <f>_xlfn.DISPIMG("ID_A28CCF741D2F4C959572208881E29708",1)</f>
+        <v>=DISPIMG("ID_A28CCF741D2F4C959572208881E29708",1)</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="N9"/>
+    </row>
+    <row r="10" ht="71" customHeight="1" spans="1:14">
+      <c r="A10" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="27" t="str">
         <f>_xlfn.DISPIMG("ID_6763D977B250450ABFE5A7D8A1F632C1",1)</f>
         <v>=DISPIMG("ID_6763D977B250450ABFE5A7D8A1F632C1",1)</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="28" t="s">
+      <c r="C10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="N9"/>
-    </row>
-    <row r="10" ht="75" customHeight="1" spans="1:14">
-      <c r="A10" s="22" t="s">
+      <c r="D10" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="27" t="str">
-        <f>_xlfn.DISPIMG("ID_A28CCF741D2F4C959572208881E29708",1)</f>
-        <v>=DISPIMG("ID_A28CCF741D2F4C959572208881E29708",1)</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" s="22" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="28"/>
+        <v>63</v>
+      </c>
       <c r="N10"/>
     </row>
-    <row r="11" ht="75.75" spans="1:14">
+    <row r="11" ht="85" customHeight="1" spans="1:6">
       <c r="A11" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="B11" s="27" t="str">
+        <f>_xlfn.DISPIMG("ID_163A9240D4EF485292D7AE5FEFA9852F",1)</f>
+        <v>=DISPIMG("ID_163A9240D4EF485292D7AE5FEFA9852F",1)</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" ht="75" customHeight="1" spans="1:14">
+      <c r="A12" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="27" t="str">
+        <f>_xlfn.DISPIMG("ID_7ED09DD668894ABE8A725CF2D4D0029F",1)</f>
+        <v>=DISPIMG("ID_7ED09DD668894ABE8A725CF2D4D0029F",1)</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="N12"/>
+    </row>
+    <row r="13" ht="66" customHeight="1" spans="1:14">
+      <c r="A13" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="27" t="str">
+        <f>_xlfn.DISPIMG("ID_D36F8EAEDC3D4A2D9DDF24AE96ABB005",1)</f>
+        <v>=DISPIMG("ID_D36F8EAEDC3D4A2D9DDF24AE96ABB005",1)</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13"/>
+    </row>
+    <row r="14" ht="75" customHeight="1" spans="1:14">
+      <c r="A14" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="27" t="str">
+        <f>_xlfn.DISPIMG("ID_A046AFD9A3BF492EADA57F8350871DB2",1)</f>
+        <v>=DISPIMG("ID_A046AFD9A3BF492EADA57F8350871DB2",1)</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="N14"/>
+    </row>
+    <row r="15" ht="75" customHeight="1" spans="1:14">
+      <c r="A15" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="27" t="str">
+        <f>_xlfn.DISPIMG("ID_2AC053A6DE184E4097DCE1BD0082E519",1)</f>
+        <v>=DISPIMG("ID_2AC053A6DE184E4097DCE1BD0082E519",1)</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="28"/>
+      <c r="N15"/>
+    </row>
+    <row r="16" ht="75" customHeight="1" spans="1:14">
+      <c r="A16" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="27" t="str">
+        <f>_xlfn.DISPIMG("ID_D72C5AF664FF4D6C8BB8BF8BE922256D",1)</f>
+        <v>=DISPIMG("ID_D72C5AF664FF4D6C8BB8BF8BE922256D",1)</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="N16"/>
+    </row>
+    <row r="17" ht="75" customHeight="1" spans="2:14">
+      <c r="B17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="N17"/>
+    </row>
+    <row r="18" ht="75" customHeight="1" spans="2:14">
+      <c r="B18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="N18"/>
+    </row>
+    <row r="19" ht="75" customHeight="1" spans="2:14">
+      <c r="B19" s="27"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="N19"/>
+    </row>
+    <row r="20" ht="75" customHeight="1" spans="2:14">
+      <c r="B20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="N20"/>
+    </row>
+    <row r="21" ht="75.75" spans="1:14">
+      <c r="A21" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="N21"/>
+    </row>
+    <row r="22" ht="56.25" spans="1:14">
+      <c r="A22" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="N23"/>
+    </row>
+    <row r="24" ht="37.5" spans="1:14">
+      <c r="A24" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="N24"/>
+    </row>
+    <row r="25" ht="56.25" spans="1:14">
+      <c r="A25" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="N25"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="28" t="s">
+      <c r="C26" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="N11"/>
-    </row>
-    <row r="12" spans="14:14">
-      <c r="N12"/>
-    </row>
-    <row r="13" ht="66" customHeight="1" spans="14:14">
-      <c r="N13"/>
-    </row>
-    <row r="14" spans="14:14">
-      <c r="N14"/>
-    </row>
-    <row r="15" ht="56.25" spans="1:14">
-      <c r="A15" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="N15"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="22" t="s">
+      <c r="D26" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" ht="56.25" spans="1:6">
+      <c r="A27" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="N16"/>
-    </row>
-    <row r="17" ht="37.5" spans="1:14">
-      <c r="A17" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="N17"/>
-    </row>
-    <row r="18" ht="56.25" spans="1:14">
-      <c r="A18" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="N18"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" ht="56.25" spans="1:6">
-      <c r="A20" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" ht="93.75" spans="1:8">
-      <c r="A21" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" ht="37.5" spans="1:8">
-      <c r="A22" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" ht="37.5" spans="1:8">
-      <c r="A23" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" ht="37.5" spans="1:7">
-      <c r="A24" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="22" t="s">
+      <c r="F27" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="28" t="s">
+    </row>
+    <row r="28" ht="56.25" spans="1:8">
+      <c r="A28" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="C28" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="22" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="25" ht="56.25" spans="1:8">
-      <c r="A25" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="G25" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" ht="37.5" spans="1:13">
-      <c r="A26" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="G26" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="K26" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="L26" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="M26" s="34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" ht="56.25" spans="1:13">
-      <c r="A27" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="G27" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="K27" s="35">
-        <v>1</v>
-      </c>
-      <c r="L27" s="36">
-        <v>15</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" ht="37.5" spans="1:13">
-      <c r="A28" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>125</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" ht="37.5" spans="1:8">
+      <c r="A29" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" ht="37.5" spans="1:8">
+      <c r="A30" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" ht="37.5" spans="1:7">
+      <c r="A31" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G31" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="H28" s="28" t="s">
+    </row>
+    <row r="32" ht="56.25" spans="1:8">
+      <c r="A32" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="K28" s="35">
+      <c r="C32" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" ht="37.5" spans="1:13">
+      <c r="A33" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="L28" s="37">
+      <c r="M33" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" ht="56.25" spans="1:13">
+      <c r="A34" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="K34" s="35">
+        <v>1</v>
+      </c>
+      <c r="L34" s="36">
+        <v>15</v>
+      </c>
+      <c r="M34" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" ht="37.5" spans="1:13">
+      <c r="A35" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="K35" s="35">
+        <v>2</v>
+      </c>
+      <c r="L35" s="37">
         <v>21</v>
       </c>
-      <c r="M28" s="22" t="s">
+      <c r="M35" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" ht="37.5" spans="1:13">
-      <c r="A29" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="K29" s="35">
+    <row r="36" ht="37.5" spans="1:13">
+      <c r="A36" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="K36" s="35">
         <v>3</v>
       </c>
-      <c r="L29" s="37">
+      <c r="L36" s="37">
         <v>27</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M36" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" ht="56.25" spans="1:13">
-      <c r="A30" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="E30" s="28" t="s">
+    <row r="37" ht="56.25" spans="1:13">
+      <c r="A37" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="F30" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="K30" s="35">
+      <c r="D37" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="K37" s="35">
         <v>4</v>
       </c>
-      <c r="L30" s="37">
+      <c r="L37" s="37">
         <v>33</v>
       </c>
-      <c r="M30" s="22" t="s">
+      <c r="M37" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" ht="37.5" spans="1:13">
-      <c r="A31" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="H31" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="K31" s="35">
+    <row r="38" ht="37.5" spans="1:13">
+      <c r="A38" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="K38" s="35">
         <v>5</v>
       </c>
-      <c r="L31" s="37">
+      <c r="L38" s="37">
         <v>39</v>
       </c>
-      <c r="M31" s="22" t="s">
+      <c r="M38" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" ht="37.5" spans="1:13">
-      <c r="A32" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="E32" s="22" t="s">
+    <row r="39" ht="37.5" spans="1:13">
+      <c r="A39" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="K32" s="35">
+      <c r="F39" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="K39" s="35">
         <v>6</v>
       </c>
-      <c r="L32" s="37">
+      <c r="L39" s="37">
         <v>45</v>
       </c>
-      <c r="M32" s="22" t="s">
+      <c r="M39" s="22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" ht="37.5" spans="1:13">
-      <c r="A33" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="B33" s="28"/>
-      <c r="K33" s="35">
+    <row r="40" ht="37.5" spans="1:13">
+      <c r="A40" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" s="28"/>
+      <c r="K40" s="35">
         <v>7</v>
       </c>
-      <c r="L33" s="37">
+      <c r="L40" s="37">
         <v>51</v>
       </c>
-      <c r="M33" s="22" t="s">
+      <c r="M40" s="22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="K34" s="35">
+    <row r="41" spans="1:13">
+      <c r="A41" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="K41" s="35">
         <v>8</v>
       </c>
-      <c r="L34" s="37">
+      <c r="L41" s="37">
         <v>57</v>
       </c>
-      <c r="M34" s="22" t="s">
+      <c r="M41" s="22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="K35" s="35">
+    <row r="42" spans="1:13">
+      <c r="A42" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="K42" s="35">
         <v>9</v>
       </c>
-      <c r="L35" s="37">
+      <c r="L42" s="37">
         <v>63</v>
       </c>
-      <c r="M35" s="22" t="s">
+      <c r="M42" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="F36" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="K36" s="38">
+    <row r="43" spans="1:13">
+      <c r="A43" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="K43" s="38">
         <v>10</v>
       </c>
-      <c r="L36" s="39">
+      <c r="L43" s="39">
         <v>69</v>
       </c>
-      <c r="M36" s="40" t="s">
+      <c r="M43" s="40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>147</v>
+    <row r="44" spans="1:6">
+      <c r="A44" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -5280,7 +5659,7 @@
   <dimension ref="B3:H11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="7"/>
@@ -5300,37 +5679,37 @@
   <sheetData>
     <row r="3" spans="2:8">
       <c r="B3" s="14" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" ht="65.55" customHeight="1" spans="2:7">
       <c r="B4" s="1" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</f>
         <v>=DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="G4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_2440730E3B794D249A4BBFB68234E0A5",1)</f>
@@ -5339,39 +5718,39 @@
     </row>
     <row r="5" ht="44" customHeight="1" spans="2:8">
       <c r="B5" s="1" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</f>
         <v>=DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="G5" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</f>
         <v>=DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" ht="47" customHeight="1" spans="2:7">
       <c r="B6" s="3" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</f>
         <v>=DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="G6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_491D9B3CF8B4441CAD720B86DCA07462",1)</f>
@@ -5380,39 +5759,39 @@
     </row>
     <row r="7" ht="64" customHeight="1" spans="2:8">
       <c r="B7" s="1" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</f>
         <v>=DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="G7" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</f>
         <v>=DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" ht="40" customHeight="1" spans="2:7">
       <c r="B8" s="1" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</f>
         <v>=DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G8" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_DD37BC4AF6A646D482F166D1DA3483B9",1)</f>
@@ -5421,13 +5800,13 @@
     </row>
     <row r="9" ht="62" customHeight="1" spans="2:7">
       <c r="B9" s="1" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="G9" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_CC66E0BDF222479FBCA1D73D9EEF98C9",1)</f>
@@ -5436,7 +5815,7 @@
     </row>
     <row r="10" ht="33" customHeight="1" spans="6:7">
       <c r="F10" s="1" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="G10" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_69F91952F7254C9081725FDDC3777D6A",1)</f>
@@ -5445,14 +5824,14 @@
     </row>
     <row r="11" ht="50" customHeight="1" spans="6:8">
       <c r="F11" s="1" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="G11" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</f>
         <v>=DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -5464,10 +5843,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B9:K55"/>
+  <dimension ref="B9:K56"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -5487,46 +5866,46 @@
   <sheetData>
     <row r="9" spans="2:11">
       <c r="B9" s="14" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" ht="44" customHeight="1" spans="3:11">
       <c r="C10" s="1" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="D10" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B89FB7A8B8234D6EAF929FE5AE44207A",1)</f>
         <v>=DISPIMG("ID_B89FB7A8B8234D6EAF929FE5AE44207A",1)</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -5534,23 +5913,23 @@
     </row>
     <row r="11" ht="45" customHeight="1" spans="2:11">
       <c r="B11" s="1" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="D11" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</f>
         <v>=DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="K11" s="1">
         <v>2</v>
@@ -5558,23 +5937,23 @@
     </row>
     <row r="12" ht="56.25" spans="2:11">
       <c r="B12" s="1" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="D12" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_601DEB5433E749A5B04D3AB579BF0284",1)</f>
         <v>=DISPIMG("ID_601DEB5433E749A5B04D3AB579BF0284",1)</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="K12" s="1">
         <v>1</v>
@@ -5582,23 +5961,23 @@
     </row>
     <row r="13" ht="117" customHeight="1" spans="2:11">
       <c r="B13" s="1" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="D13" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</f>
         <v>=DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="F13" s="1">
         <v>4</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="K13" s="1">
         <v>5</v>
@@ -5606,173 +5985,166 @@
     </row>
     <row r="14" ht="112.5" spans="2:11">
       <c r="B14" s="1" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="D14" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_900DEDBC95DA49B6832F8E0EAF3922E7",1)</f>
         <v>=DISPIMG("ID_900DEDBC95DA49B6832F8E0EAF3922E7",1)</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="F14" s="1">
         <v>5</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="K14" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="15" ht="37.5" spans="2:6">
+    <row r="15" ht="117" customHeight="1" spans="2:6">
       <c r="B15" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</f>
-        <v>=DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</v>
+        <v>197</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" ht="37.5" spans="2:6">
       <c r="B16" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>198</v>
+      <c r="C16" s="17" t="s">
+        <v>213</v>
       </c>
       <c r="D16" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</f>
+        <v>=DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" ht="37.5" spans="2:6">
+      <c r="B17" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_5B5C76B37B874958A231351EBD5A6E7C",1)</f>
         <v>=DISPIMG("ID_5B5C76B37B874958A231351EBD5A6E7C",1)</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="E17" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F17" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="17" ht="75" spans="2:6">
-      <c r="B17" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D17" s="1" t="str">
+    <row r="18" ht="75" spans="2:6">
+      <c r="B18" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B7F3E8AB96A746EEA8D18747E89057C6",1)</f>
         <v>=DISPIMG("ID_B7F3E8AB96A746EEA8D18747E89057C6",1)</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="E18" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="18" ht="29.25" spans="2:6">
-      <c r="B18" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D18" s="1" t="str">
+    <row r="19" ht="29.25" spans="2:6">
+      <c r="B19" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_05B2EF6AB8B64DED9EE5B9B0C23F991B",1)</f>
         <v>=DISPIMG("ID_05B2EF6AB8B64DED9EE5B9B0C23F991B",1)</v>
       </c>
-      <c r="E18" s="67" t="s">
-        <v>203</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" ht="37.5" spans="2:6">
-      <c r="B19" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D19" s="1" t="str">
+      <c r="E19" s="67" t="s">
+        <v>221</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" ht="37.5" spans="2:6">
+      <c r="B20" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_52D5A41E637044A490A457D53A6E6968",1)</f>
         <v>=DISPIMG("ID_52D5A41E637044A490A457D53A6E6968",1)</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F19" s="1">
+      <c r="E20" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F20" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="20" ht="93.75" spans="2:6">
-      <c r="B20" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D20" s="1" t="str">
+    <row r="21" ht="93.75" spans="2:6">
+      <c r="B21" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3B6DDDD98A8F40BC81817AB7D481E31C",1)</f>
         <v>=DISPIMG("ID_3B6DDDD98A8F40BC81817AB7D481E31C",1)</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="E21" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F21" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="21" ht="56.25" spans="2:9">
-      <c r="B21" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D21" s="1" t="str">
+    <row r="22" ht="56.25" spans="2:9">
+      <c r="B22" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_9DEEB880DCB04491A4378D1013CB4998",1)</f>
         <v>=DISPIMG("ID_9DEEB880DCB04491A4378D1013CB4998",1)</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="E22" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="F22" s="1">
         <v>4</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" ht="93.75" spans="2:9">
-      <c r="B22" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D22" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</f>
-        <v>=DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F22" s="1">
-        <v>3</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -5780,255 +6152,262 @@
     </row>
     <row r="23" ht="93.75" spans="2:9">
       <c r="B23" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>211</v>
+        <v>215</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</f>
+        <v>=DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>196</v>
+        <v>228</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" ht="56.25" spans="2:6">
+    <row r="24" ht="93.75" spans="2:9">
       <c r="B24" s="1" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="D24" s="1" t="str">
+        <v>229</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" ht="56.25" spans="2:6">
+      <c r="B25" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D25" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3597ED710A4940C9B87FCDF5F4476A1D",1)</f>
         <v>=DISPIMG("ID_3597ED710A4940C9B87FCDF5F4476A1D",1)</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C25" s="17" t="s">
+      <c r="E25" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="26" ht="37.5" spans="2:6">
-      <c r="B26" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>218</v>
+      <c r="C26" s="17" t="s">
+        <v>233</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="F26" s="1">
+        <v>234</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" ht="37.5" spans="2:6">
+      <c r="B27" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F27" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="27" ht="56.25" spans="2:6">
-      <c r="B27" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="F27" s="1">
+    <row r="28" ht="56.25" spans="2:6">
+      <c r="B28" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F28" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="28" ht="37.5" spans="2:6">
-      <c r="B28" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F28" s="1">
+    <row r="29" ht="37.5" spans="2:6">
+      <c r="B29" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F29" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="29" ht="75" spans="2:6">
-      <c r="B29" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="F29" s="1">
+    <row r="30" ht="75" spans="2:6">
+      <c r="B30" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F30" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="30" ht="93.75" spans="2:6">
-      <c r="B30" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="F30" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
+    <row r="31" ht="93.75" spans="2:6">
       <c r="B31" s="1" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>229</v>
+        <v>244</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="F31" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="32" ht="56.25" spans="2:6">
+    <row r="32" spans="2:6">
       <c r="B32" s="1" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>231</v>
+        <v>246</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="F32" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" ht="37.5" spans="2:6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" ht="56.25" spans="2:6">
       <c r="B33" s="1" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="F33" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="34" ht="56.25" spans="2:6">
+    <row r="34" ht="37.5" spans="2:6">
       <c r="B34" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>234</v>
+        <v>235</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" ht="56.25" spans="2:6">
+      <c r="B35" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F34" s="1">
+      <c r="C35" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F35" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="35" ht="93.75" spans="2:5">
-      <c r="B35" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
+    <row r="36" ht="93.75" spans="2:5">
       <c r="B36" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>216</v>
+        <v>235</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>179</v>
+        <v>256</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F37" s="1">
+        <v>234</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" s="1">
         <v>0</v>
-      </c>
-    </row>
-    <row r="38" ht="37.5" spans="2:6">
-      <c r="B38" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="F38" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="39" ht="37.5" spans="2:6">
       <c r="B39" s="1" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="F39" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" ht="93.75" spans="2:6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" ht="37.5" spans="2:6">
       <c r="B40" s="1" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="F40" s="1">
         <v>3</v>
@@ -6036,215 +6415,229 @@
     </row>
     <row r="41" ht="93.75" spans="2:6">
       <c r="B41" s="1" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="F41" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" ht="93.75" spans="2:6">
+      <c r="B42" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F42" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
-      <c r="B42" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="43" ht="75" spans="2:6">
+    <row r="43" spans="2:6">
       <c r="B43" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="F43" s="1">
+        <v>257</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="44" ht="75" spans="2:6">
+      <c r="B44" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F44" s="1">
         <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="B44" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="1" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" ht="56.25" spans="2:6">
-      <c r="B46" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>253</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="F46" s="1">
-        <v>5</v>
+        <v>234</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="47" ht="56.25" spans="2:6">
-      <c r="B47" s="1" t="s">
-        <v>255</v>
+      <c r="B47" s="3" t="s">
+        <v>270</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="F47" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="48" ht="37.5" spans="2:6">
+    <row r="48" ht="56.25" spans="2:6">
       <c r="B48" s="1" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="F48" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" ht="37.5" spans="2:6">
+      <c r="B49" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F49" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="49" ht="75" spans="2:6">
-      <c r="B49" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="F49" s="1">
+    <row r="50" ht="75" spans="2:6">
+      <c r="B50" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F50" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="50" ht="56.25" spans="2:6">
-      <c r="B50" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="F50" s="1">
+    <row r="51" ht="56.25" spans="2:6">
+      <c r="B51" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="F51" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="51" ht="56.25" spans="2:6">
-      <c r="B51" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="F51" s="1">
-        <v>6</v>
-      </c>
-    </row>
     <row r="52" ht="56.25" spans="2:6">
-      <c r="B52" s="1" t="s">
-        <v>269</v>
+      <c r="B52" s="3" t="s">
+        <v>284</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F52" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="53" ht="37.5" spans="2:6">
+    <row r="53" ht="56.25" spans="2:6">
       <c r="B53" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>273</v>
+        <v>287</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>288</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="54" ht="75" spans="2:6">
-      <c r="B54" s="3" t="s">
-        <v>275</v>
+        <v>289</v>
+      </c>
+      <c r="F53" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" ht="37.5" spans="2:6">
+      <c r="B54" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7">
-      <c r="B55" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F55" s="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" ht="75" spans="2:6">
+      <c r="B55" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="B56" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F56" s="1">
         <v>1</v>
       </c>
-      <c r="G55" s="13" t="s">
-        <v>280</v>
+      <c r="G56" s="13" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -6259,7 +6652,7 @@
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -6279,7 +6672,7 @@
   <sheetData>
     <row r="2" ht="30" customHeight="1" spans="2:6">
       <c r="B2" s="4" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -6288,73 +6681,73 @@
     </row>
     <row r="3" ht="38.25" spans="2:4">
       <c r="B3" s="7" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" ht="57" spans="2:6">
       <c r="B4" s="8" t="s">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" ht="38.25" spans="2:6">
       <c r="B5" s="2" t="s">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" ht="84" customHeight="1" spans="2:6">
       <c r="B6" s="2" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" ht="19.5" spans="2:10">
       <c r="B8" s="9" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -6367,28 +6760,28 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="D9" s="1">
         <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>308</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" ht="38.25" spans="2:7">
@@ -6396,19 +6789,19 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>310</v>
+        <v>328</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>311</v>
+        <v>329</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>313</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -6427,7 +6820,7 @@
   <dimension ref="B2:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -6441,13 +6834,13 @@
   <sheetData>
     <row r="2" ht="81" customHeight="1" spans="2:4">
       <c r="B2" s="2" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>314</v>
+        <v>332</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Locked Chest event and Natas event. Created the sprites for Sandman. Added 2 more AI's: scared and restless. Natas still WIP
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12495" activeTab="1"/>
+    <workbookView windowWidth="23295" windowHeight="13095" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -1093,7 +1093,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="337">
   <si>
     <t>Player Level</t>
   </si>
@@ -2275,6 +2275,17 @@
     <t>Use to trigger traps and stuff</t>
   </si>
   <si>
+    <t>Rogue, Ranger</t>
+  </si>
+  <si>
+    <t>Pick Lock</t>
+  </si>
+  <si>
+    <t>Locks become REALLY
+easy to pick, like come on...
+You also get extra treasure</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -2437,8 +2448,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="31">
@@ -2534,17 +2545,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2565,15 +2575,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2582,14 +2601,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2612,7 +2623,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2626,16 +2653,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2650,14 +2676,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2665,14 +2684,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2687,7 +2698,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2705,7 +2746,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2717,25 +2848,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2747,103 +2866,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2855,19 +2878,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3186,21 +3197,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -3211,6 +3207,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3239,20 +3255,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3274,11 +3287,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3287,15 +3298,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -3305,130 +3316,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4686,8 +4697,8 @@
   <sheetPr/>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
@@ -5843,10 +5854,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B9:K56"/>
+  <dimension ref="B9:K57"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -5857,8 +5868,9 @@
     <col min="4" max="4" width="15.8571428571429" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.8571428571429" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.5714285714286" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.9428571428571" style="13" customWidth="1"/>
-    <col min="8" max="9" width="9.14285714285714" style="13"/>
+    <col min="7" max="7" width="34.4" style="13" customWidth="1"/>
+    <col min="8" max="8" width="18.6285714285714" style="13" customWidth="1"/>
+    <col min="9" max="9" width="9.14285714285714" style="13"/>
     <col min="10" max="10" width="18.8571428571429" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.8571428571429" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.14285714285714" style="13"/>
@@ -6623,7 +6635,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" ht="39" customHeight="1" spans="2:7">
       <c r="B56" s="1" t="s">
         <v>290</v>
       </c>
@@ -6638,6 +6650,17 @@
       </c>
       <c r="G56" s="13" t="s">
         <v>298</v>
+      </c>
+    </row>
+    <row r="57" ht="112.5" spans="2:5">
+      <c r="B57" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -6672,7 +6695,7 @@
   <sheetData>
     <row r="2" ht="30" customHeight="1" spans="2:6">
       <c r="B2" s="4" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -6681,73 +6704,73 @@
     </row>
     <row r="3" ht="38.25" spans="2:4">
       <c r="B3" s="7" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" ht="57" spans="2:6">
       <c r="B4" s="8" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" ht="38.25" spans="2:6">
       <c r="B5" s="2" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" ht="84" customHeight="1" spans="2:6">
       <c r="B6" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" ht="19.5" spans="2:10">
       <c r="B8" s="9" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -6760,28 +6783,28 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D9" s="1">
         <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" ht="38.25" spans="2:7">
@@ -6789,19 +6812,19 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -6837,10 +6860,10 @@
         <v>201</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed tons of buggs. Added Throw Net to Peasants, Mermaids and Driders. Also added a version of Throw Net to Ranger, which is a default ability. Added scrolling text for most effects, heals, blocks, mana gains, etc. Highwaymen now have a targeted ability which an be partially blocked by standing behind another unit. Reworked zombies. They now have a normal attack which drains stats.
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23295" windowHeight="13095" activeTab="3"/>
+    <workbookView windowWidth="23295" windowHeight="13095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -2270,7 +2270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="456">
   <si>
     <t>Player Level</t>
   </si>
@@ -2401,6 +2401,9 @@
 ground there</t>
   </si>
   <si>
+    <t>50% chance to hit a player</t>
+  </si>
+  <si>
     <t>Killable in 1 + 2 shot</t>
   </si>
   <si>
@@ -2447,6 +2450,9 @@
   </si>
   <si>
     <t>Goes dormant if stuck</t>
+  </si>
+  <si>
+    <t>On death, infects all nearby units</t>
   </si>
   <si>
     <t>Evil Paprika</t>
@@ -4000,10 +4006,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -4104,18 +4110,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4126,9 +4133,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4145,20 +4151,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4187,6 +4179,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -4197,14 +4197,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4227,15 +4234,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4257,7 +4263,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4269,31 +4287,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4305,19 +4305,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4329,25 +4323,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4365,13 +4341,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4383,7 +4353,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4401,31 +4383,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4438,6 +4402,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4755,6 +4761,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -4766,15 +4781,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4805,9 +4811,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4844,11 +4852,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4857,148 +4863,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6268,10 +6274,10 @@
   <sheetPr/>
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -6407,14 +6413,17 @@
       <c r="F5" s="24" t="s">
         <v>41</v>
       </c>
+      <c r="G5" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="I5" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N5"/>
     </row>
     <row r="6" ht="58" customHeight="1" spans="1:14">
       <c r="A6" s="23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_5DCB40CCA6B44244B7519B2BA06EDF1C",1)</f>
@@ -6427,16 +6436,16 @@
         <v>32</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N6"/>
     </row>
     <row r="7" ht="68" customHeight="1" spans="1:14">
       <c r="A7" s="23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B7" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_48D844B5BD4E47F1A264B90859DAC1E8",1)</f>
@@ -6446,25 +6455,25 @@
         <v>32</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E7" s="23" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N7"/>
     </row>
     <row r="8" ht="71" customHeight="1" spans="1:14">
       <c r="A8" s="30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8" s="31" t="str">
         <f>_xlfn.DISPIMG("ID_9997CD209D774EEAB420C53DDEA056A0",1)</f>
@@ -6474,22 +6483,22 @@
         <v>32</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N8"/>
     </row>
     <row r="9" ht="75" customHeight="1" spans="1:14">
       <c r="A9" s="23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_A28CCF741D2F4C959572208881E29708",1)</f>
@@ -6505,530 +6514,533 @@
         <v>29</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>59</v>
       </c>
       <c r="I9" s="24"/>
       <c r="N9"/>
     </row>
     <row r="10" ht="71" customHeight="1" spans="1:14">
       <c r="A10" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B10" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_6763D977B250450ABFE5A7D8A1F632C1",1)</f>
         <v>=DISPIMG("ID_6763D977B250450ABFE5A7D8A1F632C1",1)</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N10"/>
     </row>
     <row r="11" ht="85" customHeight="1" spans="1:6">
       <c r="A11" s="23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B11" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_163A9240D4EF485292D7AE5FEFA9852F",1)</f>
         <v>=DISPIMG("ID_163A9240D4EF485292D7AE5FEFA9852F",1)</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" ht="75" customHeight="1" spans="1:14">
       <c r="A12" s="23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B12" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_7ED09DD668894ABE8A725CF2D4D0029F",1)</f>
         <v>=DISPIMG("ID_7ED09DD668894ABE8A725CF2D4D0029F",1)</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N12"/>
     </row>
     <row r="13" ht="66" customHeight="1" spans="1:14">
       <c r="A13" s="23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B13" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_D36F8EAEDC3D4A2D9DDF24AE96ABB005",1)</f>
         <v>=DISPIMG("ID_D36F8EAEDC3D4A2D9DDF24AE96ABB005",1)</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N13"/>
     </row>
     <row r="14" ht="75" customHeight="1" spans="1:14">
       <c r="A14" s="23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B14" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_A046AFD9A3BF492EADA57F8350871DB2",1)</f>
         <v>=DISPIMG("ID_A046AFD9A3BF492EADA57F8350871DB2",1)</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="N14"/>
     </row>
     <row r="15" ht="75" customHeight="1" spans="1:14">
       <c r="A15" s="23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B15" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_2AC053A6DE184E4097DCE1BD0082E519",1)</f>
         <v>=DISPIMG("ID_2AC053A6DE184E4097DCE1BD0082E519",1)</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="N15"/>
     </row>
     <row r="16" ht="75" customHeight="1" spans="1:14">
       <c r="A16" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B16" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_D72C5AF664FF4D6C8BB8BF8BE922256D",1)</f>
         <v>=DISPIMG("ID_D72C5AF664FF4D6C8BB8BF8BE922256D",1)</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N16"/>
     </row>
     <row r="17" ht="75" customHeight="1" spans="1:14">
       <c r="A17" s="23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B17" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_8F384D93F8A041A7BCCE76056201BF0F",1)</f>
         <v>=DISPIMG("ID_8F384D93F8A041A7BCCE76056201BF0F",1)</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="N17"/>
     </row>
     <row r="18" ht="75" customHeight="1" spans="1:14">
       <c r="A18" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B18" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_096FB0EDD1054600AEE93DB32445E432",1)</f>
         <v>=DISPIMG("ID_096FB0EDD1054600AEE93DB32445E432",1)</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N18"/>
     </row>
     <row r="19" ht="75" customHeight="1" spans="1:14">
       <c r="A19" s="23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B19" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_FD9E219F3F5B421E997BB811EC08D139",1)</f>
         <v>=DISPIMG("ID_FD9E219F3F5B421E997BB811EC08D139",1)</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N19"/>
     </row>
     <row r="20" ht="75" customHeight="1" spans="1:14">
       <c r="A20" s="23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B20" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_8A4C0CA2B27A4C878CAEF5F7F6D84956",1)</f>
         <v>=DISPIMG("ID_8A4C0CA2B27A4C878CAEF5F7F6D84956",1)</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="N20"/>
     </row>
     <row r="21" ht="75" customHeight="1" spans="1:14">
       <c r="A21" s="23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B21" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_F8B9634EB73D4F649475A0DA1DCAE550",1)</f>
         <v>=DISPIMG("ID_F8B9634EB73D4F649475A0DA1DCAE550",1)</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="N21"/>
     </row>
     <row r="22" ht="45" customHeight="1" spans="1:14">
       <c r="A22" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B22" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_53946E75DFA2463A9C5A11C27661E786",1)</f>
         <v>=DISPIMG("ID_53946E75DFA2463A9C5A11C27661E786",1)</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N22"/>
     </row>
     <row r="23" ht="75" customHeight="1" spans="1:14">
       <c r="A23" s="23" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B23" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_A9D352B95303458B89C1717F79CDE735",1)</f>
         <v>=DISPIMG("ID_A9D352B95303458B89C1717F79CDE735",1)</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="N23"/>
     </row>
     <row r="24" ht="75" customHeight="1" spans="1:14">
       <c r="A24" s="23" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B24" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_E06E036609E94BB9929FE03D33A7B60B",1)</f>
         <v>=DISPIMG("ID_E06E036609E94BB9929FE03D33A7B60B",1)</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N24"/>
     </row>
     <row r="25" ht="75" customHeight="1" spans="1:14">
       <c r="A25" s="23" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B25" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_904652B47CF844A8B4968D95A64E3891",1)</f>
         <v>=DISPIMG("ID_904652B47CF844A8B4968D95A64E3891",1)</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="N25"/>
     </row>
     <row r="26" ht="75" customHeight="1" spans="1:14">
       <c r="A26" s="23" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B26" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_C711069D368A4C1E9B8B5E98151EADAC",1)</f>
         <v>=DISPIMG("ID_C711069D368A4C1E9B8B5E98151EADAC",1)</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="N26"/>
     </row>
     <row r="27" ht="75" customHeight="1" spans="1:14">
       <c r="A27" s="23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B27" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_6C082183216B495085F7DBF1E3D99F5E",1)</f>
         <v>=DISPIMG("ID_6C082183216B495085F7DBF1E3D99F5E",1)</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>39</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N27"/>
     </row>
     <row r="28" ht="75" customHeight="1" spans="1:14">
       <c r="A28" s="23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B28" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_628E96F4BF42434FA277775E1DE2AA20",1)</f>
         <v>=DISPIMG("ID_628E96F4BF42434FA277775E1DE2AA20",1)</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="N28"/>
     </row>
     <row r="29" ht="75" customHeight="1" spans="1:14">
       <c r="A29" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B29" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_B9BED2D4AE354012A6BAB6A7E0FF5802",1)</f>
         <v>=DISPIMG("ID_B9BED2D4AE354012A6BAB6A7E0FF5802",1)</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="N29"/>
     </row>
     <row r="30" ht="75" customHeight="1" spans="1:14">
       <c r="A30" s="30" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B30" s="31" t="str">
         <f>_xlfn.DISPIMG("ID_7A9E03A399CC4F74B895A88C9005BB92",1)</f>
         <v>=DISPIMG("ID_7A9E03A399CC4F74B895A88C9005BB92",1)</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N30"/>
     </row>
     <row r="31" ht="75" customHeight="1" spans="1:14">
       <c r="A31" s="23" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B31" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_65FDB7CD50CF472E9EE58BDBA9A1B3FA",1)</f>
         <v>=DISPIMG("ID_65FDB7CD50CF472E9EE58BDBA9A1B3FA",1)</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N31"/>
     </row>
@@ -7038,255 +7050,255 @@
     </row>
     <row r="33" ht="75" customHeight="1" spans="1:14">
       <c r="A33" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B33" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_AFFBB67C163A41AA92F2B00342A712D5",1)</f>
         <v>=DISPIMG("ID_AFFBB67C163A41AA92F2B00342A712D5",1)</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N33"/>
     </row>
     <row r="34" ht="75" customHeight="1" spans="1:14">
       <c r="A34" s="23" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B34" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_A2CCFFC477CB41C68B5C4B028618A131",1)</f>
         <v>=DISPIMG("ID_A2CCFFC477CB41C68B5C4B028618A131",1)</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N34"/>
     </row>
     <row r="35" ht="75" customHeight="1" spans="1:14">
       <c r="A35" s="23" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B35" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_83BCD919FA48483A8504C30F86775227",1)</f>
         <v>=DISPIMG("ID_83BCD919FA48483A8504C30F86775227",1)</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N35"/>
     </row>
     <row r="36" ht="75" customHeight="1" spans="1:14">
       <c r="A36" s="23" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B36" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_F6C581482AFC49CF88B4B51DB4C2B884",1)</f>
         <v>=DISPIMG("ID_F6C581482AFC49CF88B4B51DB4C2B884",1)</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="N36"/>
     </row>
     <row r="37" ht="75" customHeight="1" spans="1:14">
       <c r="A37" s="23" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B37" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_B56FE51048C84C21B0544EC1D2B49BFB",1)</f>
         <v>=DISPIMG("ID_B56FE51048C84C21B0544EC1D2B49BFB",1)</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="N37"/>
     </row>
     <row r="38" ht="75" customHeight="1" spans="1:14">
       <c r="A38" s="23" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B38" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_2BF7160B000D4507A9BC6E9CD0CFBB9A",1)</f>
         <v>=DISPIMG("ID_2BF7160B000D4507A9BC6E9CD0CFBB9A",1)</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N38"/>
     </row>
     <row r="39" ht="75" customHeight="1" spans="1:14">
       <c r="A39" s="23" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B39" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_F51C6D32B5FE4CB4BAE5E9D1DF1B99A4",1)</f>
         <v>=DISPIMG("ID_F51C6D32B5FE4CB4BAE5E9D1DF1B99A4",1)</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N39"/>
     </row>
     <row r="40" ht="75" customHeight="1" spans="1:14">
       <c r="A40" s="23" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B40" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_42E1FCCA38754E91AC4BDE1CCF581E79",1)</f>
         <v>=DISPIMG("ID_42E1FCCA38754E91AC4BDE1CCF581E79",1)</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H40" s="24" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N40"/>
     </row>
     <row r="41" ht="75" customHeight="1" spans="1:14">
       <c r="A41" s="23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B41" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_FCC8AFB7F83C4286AEE68D9A89ABD31C",1)</f>
         <v>=DISPIMG("ID_FCC8AFB7F83C4286AEE68D9A89ABD31C",1)</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="N41"/>
     </row>
     <row r="42" ht="75" customHeight="1" spans="1:14">
       <c r="A42" s="23" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B42" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_28ECA6BF9B5F4B8AB2A28048D7A7B8D6",1)</f>
         <v>=DISPIMG("ID_28ECA6BF9B5F4B8AB2A28048D7A7B8D6",1)</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="N42"/>
     </row>
     <row r="43" ht="75" customHeight="1" spans="1:14">
       <c r="A43" s="23" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B43" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_4F83562294774CE1B91320A1884FEEA6",1)</f>
         <v>=DISPIMG("ID_4F83562294774CE1B91320A1884FEEA6",1)</v>
       </c>
       <c r="F43" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" s="24" t="s">
         <v>166</v>
-      </c>
-      <c r="G43" s="24" t="s">
-        <v>164</v>
       </c>
       <c r="N43"/>
     </row>
     <row r="44" ht="75" customHeight="1" spans="1:14">
       <c r="A44" s="23" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B44" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_50AEDFD4C9CB4FD09CD7DBAA4E44C1E5",1)</f>
         <v>=DISPIMG("ID_50AEDFD4C9CB4FD09CD7DBAA4E44C1E5",1)</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="N44"/>
     </row>
     <row r="45" ht="75" customHeight="1" spans="1:14">
       <c r="A45" s="23" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B45" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_7FEFC25B5DDF45199372FEC1ECD4F0DB",1)</f>
         <v>=DISPIMG("ID_7FEFC25B5DDF45199372FEC1ECD4F0DB",1)</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J45" s="24" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="N45"/>
     </row>
     <row r="46" ht="75" customHeight="1" spans="1:14">
       <c r="A46" s="23" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B46" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_563C63C9B19047BAA87384017A514719",1)</f>
         <v>=DISPIMG("ID_563C63C9B19047BAA87384017A514719",1)</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="N46"/>
     </row>
@@ -7296,22 +7308,22 @@
     </row>
     <row r="48" ht="75.75" spans="1:14">
       <c r="A48" s="23" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E48" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H48" s="33"/>
       <c r="I48" s="35"/>
@@ -7319,258 +7331,258 @@
     </row>
     <row r="49" ht="56.25" spans="1:14">
       <c r="A49" s="23" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="N49"/>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="23" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E50" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="N50"/>
     </row>
     <row r="51" ht="37.5" spans="1:14">
       <c r="A51" s="23" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E51" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="N51"/>
     </row>
     <row r="52" ht="56.25" spans="1:14">
       <c r="A52" s="23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E52" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="N52"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" ht="56.25" spans="1:6">
       <c r="A54" s="23" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E54" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" ht="56.25" spans="1:8">
       <c r="A55" s="23" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E55" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H55" s="24" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="56" ht="37.5" spans="1:8">
       <c r="A56" s="23" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E56" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G56" s="24" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H56" s="24" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" ht="37.5" spans="1:8">
       <c r="A57" s="23" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E57" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H57" s="24" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" ht="37.5" spans="1:7">
       <c r="A58" s="23" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E58" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59" ht="56.25" spans="1:8">
       <c r="A59" s="23" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E59" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="H59" s="24" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" ht="37.5" spans="1:13">
       <c r="A60" s="23" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E60" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G60" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K60" s="34" t="s">
         <v>7</v>
@@ -7584,22 +7596,22 @@
     </row>
     <row r="61" ht="56.25" spans="1:13">
       <c r="A61" s="23" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E61" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="G61" s="24" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="K61" s="38">
         <v>1</v>
@@ -7613,25 +7625,25 @@
     </row>
     <row r="62" ht="37.5" spans="1:13">
       <c r="A62" s="23" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E62" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H62" s="24" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K62" s="38">
         <v>2</v>
@@ -7645,19 +7657,19 @@
     </row>
     <row r="63" ht="37.5" spans="1:13">
       <c r="A63" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K63" s="38">
         <v>3</v>
@@ -7671,19 +7683,19 @@
     </row>
     <row r="64" ht="56.25" spans="1:13">
       <c r="A64" s="23" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E64" s="24" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="K64" s="38">
         <v>4</v>
@@ -7697,25 +7709,25 @@
     </row>
     <row r="65" ht="37.5" spans="1:13">
       <c r="A65" s="23" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="K65" s="38">
         <v>5</v>
@@ -7729,19 +7741,19 @@
     </row>
     <row r="66" ht="37.5" spans="1:13">
       <c r="A66" s="23" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E66" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="K66" s="38">
         <v>6</v>
@@ -7755,7 +7767,7 @@
     </row>
     <row r="67" ht="37.5" spans="1:13">
       <c r="A67" s="24" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B67" s="24"/>
       <c r="K67" s="38">
@@ -7770,7 +7782,7 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="23" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="K68" s="38">
         <v>8</v>
@@ -7784,10 +7796,10 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="23" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="K69" s="38">
         <v>9</v>
@@ -7801,10 +7813,10 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="23" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="K70" s="41">
         <v>10</v>
@@ -7818,10 +7830,10 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="23" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -7856,37 +7868,37 @@
   <sheetData>
     <row r="3" spans="2:8">
       <c r="B3" s="14" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" ht="65.55" customHeight="1" spans="2:7">
       <c r="B4" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</f>
         <v>=DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_2440730E3B794D249A4BBFB68234E0A5",1)</f>
@@ -7895,39 +7907,39 @@
     </row>
     <row r="5" ht="44" customHeight="1" spans="2:8">
       <c r="B5" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</f>
         <v>=DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G5" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</f>
         <v>=DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" ht="47" customHeight="1" spans="2:7">
       <c r="B6" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</f>
         <v>=DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="G6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_491D9B3CF8B4441CAD720B86DCA07462",1)</f>
@@ -7936,39 +7948,39 @@
     </row>
     <row r="7" ht="64" customHeight="1" spans="2:8">
       <c r="B7" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</f>
         <v>=DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G7" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</f>
         <v>=DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" ht="40" customHeight="1" spans="2:7">
       <c r="B8" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</f>
         <v>=DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G8" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_DD37BC4AF6A646D482F166D1DA3483B9",1)</f>
@@ -7977,13 +7989,13 @@
     </row>
     <row r="9" ht="62" customHeight="1" spans="2:7">
       <c r="B9" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G9" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_CC66E0BDF222479FBCA1D73D9EEF98C9",1)</f>
@@ -7992,7 +8004,7 @@
     </row>
     <row r="10" ht="33" customHeight="1" spans="6:7">
       <c r="F10" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G10" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_69F91952F7254C9081725FDDC3777D6A",1)</f>
@@ -8001,14 +8013,14 @@
     </row>
     <row r="11" ht="50" customHeight="1" spans="6:8">
       <c r="F11" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G11" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</f>
         <v>=DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -8022,7 +8034,7 @@
   <sheetPr/>
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A18" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A18" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -8043,46 +8055,46 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="14" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>27</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" ht="44" customHeight="1" spans="2:10">
       <c r="B2" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C2" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B89FB7A8B8234D6EAF929FE5AE44207A",1)</f>
         <v>=DISPIMG("ID_B89FB7A8B8234D6EAF929FE5AE44207A",1)</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E2" s="1">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -8090,23 +8102,23 @@
     </row>
     <row r="3" ht="45" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</f>
         <v>=DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E3" s="1">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="J3" s="1">
         <v>2</v>
@@ -8114,23 +8126,23 @@
     </row>
     <row r="4" ht="29.25" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_601DEB5433E749A5B04D3AB579BF0284",1)</f>
         <v>=DISPIMG("ID_601DEB5433E749A5B04D3AB579BF0284",1)</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -8138,17 +8150,17 @@
     </row>
     <row r="5" ht="117" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_435D6C639B07467EA8A5C2BDBADEB9EF",1)</f>
         <v>=DISPIMG("ID_435D6C639B07467EA8A5C2BDBADEB9EF",1)</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
@@ -8156,17 +8168,17 @@
     </row>
     <row r="6" ht="117" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_F93D45808FD1497AA14207AA5687A0B5",1)</f>
         <v>=DISPIMG("ID_F93D45808FD1497AA14207AA5687A0B5",1)</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
@@ -8174,128 +8186,128 @@
     </row>
     <row r="7" ht="61" customHeight="1" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_BD2F4EFF81EA407EB07B30FC9A025ED8",1)</f>
         <v>=DISPIMG("ID_BD2F4EFF81EA407EB07B30FC9A025ED8",1)</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" ht="56" customHeight="1" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_6F93A133E4B345C3A8C8AB0E41048D37",1)</f>
         <v>=DISPIMG("ID_6F93A133E4B345C3A8C8AB0E41048D37",1)</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" ht="67" customHeight="1" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_9DE1483F06B1441B9301F11BB84D2728",1)</f>
         <v>=DISPIMG("ID_9DE1483F06B1441B9301F11BB84D2728",1)</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" ht="97" customHeight="1" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_E2D7BCC771AE4C57B67785698BAAC802",1)</f>
         <v>=DISPIMG("ID_E2D7BCC771AE4C57B67785698BAAC802",1)</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" ht="80" customHeight="1" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_068CF9D1A64D4B1AA847F491190CA498",1)</f>
         <v>=DISPIMG("ID_068CF9D1A64D4B1AA847F491190CA498",1)</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" ht="67" customHeight="1" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B819211F6D714CDEBBF38A9148AFAAC7",1)</f>
         <v>=DISPIMG("ID_B819211F6D714CDEBBF38A9148AFAAC7",1)</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" ht="69" customHeight="1" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_0D3B38AE54A44B3E8DF025084DB6651B",1)</f>
         <v>=DISPIMG("ID_0D3B38AE54A44B3E8DF025084DB6651B",1)</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" ht="71" customHeight="1" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</f>
         <v>=DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E14" s="1">
         <v>6</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="J14" s="1">
         <v>5</v>
@@ -8303,23 +8315,23 @@
     </row>
     <row r="15" ht="93.75" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_900DEDBC95DA49B6832F8E0EAF3922E7",1)</f>
         <v>=DISPIMG("ID_900DEDBC95DA49B6832F8E0EAF3922E7",1)</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E15" s="1">
         <v>5</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="J15" s="1">
         <v>6</v>
@@ -8327,83 +8339,83 @@
     </row>
     <row r="16" ht="117" customHeight="1" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_F1C740FD556749E1A3007CADB7F7B5AD",1)</f>
         <v>=DISPIMG("ID_F1C740FD556749E1A3007CADB7F7B5AD",1)</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" ht="53" customHeight="1" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_7295A5EE838846E9918EEC2351B4AADE",1)</f>
         <v>=DISPIMG("ID_7295A5EE838846E9918EEC2351B4AADE",1)</v>
       </c>
       <c r="D17" s="70" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" ht="70" customHeight="1" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_475395F073B348EBAD90A05DB4F70535",1)</f>
         <v>=DISPIMG("ID_475395F073B348EBAD90A05DB4F70535",1)</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" ht="37.5" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</f>
         <v>=DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" ht="37.5" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_5B5C76B37B874958A231351EBD5A6E7C",1)</f>
         <v>=DISPIMG("ID_5B5C76B37B874958A231351EBD5A6E7C",1)</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E20" s="1">
         <v>5</v>
@@ -8411,17 +8423,17 @@
     </row>
     <row r="21" ht="75" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B7F3E8AB96A746EEA8D18747E89057C6",1)</f>
         <v>=DISPIMG("ID_B7F3E8AB96A746EEA8D18747E89057C6",1)</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E21" s="1">
         <v>5</v>
@@ -8429,17 +8441,17 @@
     </row>
     <row r="22" ht="37.5" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C22" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_52D5A41E637044A490A457D53A6E6968",1)</f>
         <v>=DISPIMG("ID_52D5A41E637044A490A457D53A6E6968",1)</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E22" s="1">
         <v>8</v>
@@ -8447,17 +8459,17 @@
     </row>
     <row r="23" ht="93.75" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3B6DDDD98A8F40BC81817AB7D481E31C",1)</f>
         <v>=DISPIMG("ID_3B6DDDD98A8F40BC81817AB7D481E31C",1)</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -8465,17 +8477,17 @@
     </row>
     <row r="24" ht="56.25" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_9DEEB880DCB04491A4378D1013CB4998",1)</f>
         <v>=DISPIMG("ID_9DEEB880DCB04491A4378D1013CB4998",1)</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E24" s="1">
         <v>4</v>
@@ -8486,17 +8498,17 @@
     </row>
     <row r="25" ht="75" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</f>
         <v>=DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E25" s="1">
         <v>3</v>
@@ -8507,17 +8519,17 @@
     </row>
     <row r="26" ht="86" customHeight="1" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C26" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_FB929A3456EC484B83246B63E363119F",1)</f>
         <v>=DISPIMG("ID_FB929A3456EC484B83246B63E363119F",1)</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -8525,17 +8537,17 @@
     </row>
     <row r="27" ht="74" customHeight="1" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C27" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_CDF4F9B6AAE7428396B6B6CB350938A4",1)</f>
         <v>=DISPIMG("ID_CDF4F9B6AAE7428396B6B6CB350938A4",1)</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="E27" s="1">
         <v>8</v>
@@ -8546,17 +8558,17 @@
     </row>
     <row r="28" ht="98" customHeight="1" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C28" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_9E20CD0B9D3344AFA01653BE39E9CAED",1)</f>
         <v>=DISPIMG("ID_9E20CD0B9D3344AFA01653BE39E9CAED",1)</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E28" s="1">
         <v>4</v>
@@ -8564,56 +8576,56 @@
     </row>
     <row r="29" ht="29.25" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C29" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_05B2EF6AB8B64DED9EE5B9B0C23F991B",1)</f>
         <v>=DISPIMG("ID_05B2EF6AB8B64DED9EE5B9B0C23F991B",1)</v>
       </c>
       <c r="D29" s="71" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" ht="44" customHeight="1" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C30" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B70ADECACB0640B388DDE4A570E8A4A0",1)</f>
         <v>=DISPIMG("ID_B70ADECACB0640B388DDE4A570E8A4A0",1)</v>
       </c>
       <c r="D30" s="70" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" ht="93.75" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C31" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_F991DDDB9E524EFEA1B831F26AB76DE9",1)</f>
         <v>=DISPIMG("ID_F991DDDB9E524EFEA1B831F26AB76DE9",1)</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -8621,48 +8633,48 @@
     </row>
     <row r="32" ht="37.5" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C32" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3597ED710A4940C9B87FCDF5F4476A1D",1)</f>
         <v>=DISPIMG("ID_3597ED710A4940C9B87FCDF5F4476A1D",1)</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" ht="39" customHeight="1" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" ht="37.5" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -8670,13 +8682,13 @@
     </row>
     <row r="35" ht="56.25" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -8684,13 +8696,13 @@
     </row>
     <row r="36" ht="37.5" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E36" s="1">
         <v>3</v>
@@ -8698,13 +8710,13 @@
     </row>
     <row r="37" ht="56.25" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E37" s="1">
         <v>8</v>
@@ -8712,13 +8724,13 @@
     </row>
     <row r="38" ht="75" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="E38" s="1">
         <v>5</v>
@@ -8726,13 +8738,13 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E39" s="1">
         <v>5</v>
@@ -8740,13 +8752,13 @@
     </row>
     <row r="40" ht="56.25" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E40" s="1">
         <v>3</v>
@@ -8754,13 +8766,13 @@
     </row>
     <row r="41" ht="37.5" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E41" s="1">
         <v>3</v>
@@ -8768,13 +8780,13 @@
     </row>
     <row r="42" ht="56.25" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E42" s="1">
         <v>9</v>
@@ -8782,38 +8794,38 @@
     </row>
     <row r="43" ht="75" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -8821,13 +8833,13 @@
     </row>
     <row r="46" ht="37.5" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E46" s="1">
         <v>2</v>
@@ -8835,13 +8847,13 @@
     </row>
     <row r="47" ht="37.5" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="E47" s="1">
         <v>3</v>
@@ -8849,13 +8861,13 @@
     </row>
     <row r="48" ht="75" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E48" s="1">
         <v>3</v>
@@ -8863,13 +8875,13 @@
     </row>
     <row r="49" ht="93.75" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E49" s="1">
         <v>7</v>
@@ -8877,27 +8889,27 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="51" ht="75" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E51" s="1">
         <v>4</v>
@@ -8905,41 +8917,41 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>376</v>
-      </c>
       <c r="D52" s="3" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="54" ht="56.25" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E54" s="1">
         <v>5</v>
@@ -8947,13 +8959,13 @@
     </row>
     <row r="55" ht="56.25" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E55" s="1">
         <v>5</v>
@@ -8961,13 +8973,13 @@
     </row>
     <row r="56" ht="37.5" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E56" s="1">
         <v>6</v>
@@ -8975,13 +8987,13 @@
     </row>
     <row r="57" ht="75" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E57" s="1">
         <v>5</v>
@@ -8989,13 +9001,13 @@
     </row>
     <row r="58" ht="56.25" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="E58" s="1">
         <v>4</v>
@@ -9003,13 +9015,13 @@
     </row>
     <row r="59" ht="56.25" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="E59" s="1">
         <v>6</v>
@@ -9017,13 +9029,13 @@
     </row>
     <row r="60" ht="56.25" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="E60" s="1">
         <v>6</v>
@@ -9031,41 +9043,41 @@
     </row>
     <row r="61" ht="37.5" spans="1:5">
       <c r="A61" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62" ht="56.25" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" ht="56.25" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -9100,7 +9112,7 @@
   <sheetData>
     <row r="2" ht="30" customHeight="1" spans="2:6">
       <c r="B2" s="4" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -9109,73 +9121,73 @@
     </row>
     <row r="3" ht="38.25" spans="2:4">
       <c r="B3" s="7" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4" ht="57" spans="2:6">
       <c r="B4" s="8" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" ht="38.25" spans="2:6">
       <c r="B5" s="2" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" ht="84" customHeight="1" spans="2:6">
       <c r="B6" s="2" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" ht="19.5" spans="2:10">
       <c r="B8" s="9" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -9188,28 +9200,28 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D9" s="1">
         <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="10" ht="38.25" spans="2:7">
@@ -9217,19 +9229,19 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -9262,13 +9274,13 @@
   <sheetData>
     <row r="2" ht="81" customHeight="1" spans="2:4">
       <c r="B2" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new ability to Serfmasters and Driders (Sumo Wave). Fixed a ton of bugs and crashes.
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23295" windowHeight="13095" activeTab="1"/>
+    <workbookView windowWidth="23295" windowHeight="13095" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -2266,11 +2266,136 @@
       </xdr:spPr>
     </xdr:pic>
   </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="90" name="ID_BB4C04DA0D82463FB165645D87472EF4" descr="Throw Rock"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId89"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3138805" y="27501215"/>
+          <a:ext cx="303530" cy="310515"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="91" name="ID_38F9D2AF49AB4BCA9F11DD0853E30AF5" descr="Magic Arrow"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId90"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048635" y="28002230"/>
+          <a:ext cx="300355" cy="308610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="92" name="ID_36828F0C21034B8DBBF17DCCDA5DA267" descr="Siphon Mana"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId91"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3098165" y="28496260"/>
+          <a:ext cx="303530" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="93" name="ID_A9DB86C046194BD7BA43F0E79E4830FA" descr="Blink"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId92"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3097530" y="28966160"/>
+          <a:ext cx="304800" cy="307975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="94" name="ID_8658678BBB954416846A781790E04465" descr="Iceberg Drop"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId93"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3023235" y="29467175"/>
+          <a:ext cx="303530" cy="310515"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
 </etc:cellImages>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="459">
   <si>
     <t>Player Level</t>
   </si>
@@ -2372,6 +2497,9 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>Roots every 3 to 8 turns</t>
   </si>
   <si>
     <t>Has 6*2 + 1 HP</t>
@@ -2485,6 +2613,10 @@
 Shoots them next turn</t>
   </si>
   <si>
+    <t>Every 4 turns, shoots 3 bullets at an enemy.
+Can be partially blocked by sitting behind another unit.</t>
+  </si>
+  <si>
     <t>Guard</t>
   </si>
   <si>
@@ -2497,6 +2629,9 @@
   <si>
     <t>Attacks pierce
 and reach 2</t>
+  </si>
+  <si>
+    <t>Blocks every 2nd turn</t>
   </si>
   <si>
     <t>Rat</t>
@@ -2710,12 +2845,7 @@
     <t>Zombie</t>
   </si>
   <si>
-    <t>Can only take 1 damage at a time.</t>
-  </si>
-  <si>
-    <t>Chomp: Delayed
-Shreds Block
-Drains some mana</t>
+    <t>Attacks steal a random stat (armor, damage or MR)</t>
   </si>
   <si>
     <t>Lantern Ghoul</t>
@@ -2733,7 +2863,7 @@
     <t>Beholder</t>
   </si>
   <si>
-    <t>Attacks are Chain Ligntning and shred block</t>
+    <t>Attacks are Chain Lightning and shred block</t>
   </si>
   <si>
     <t>Attacks shred block</t>
@@ -3603,26 +3733,32 @@
     <t>Mage</t>
   </si>
   <si>
-    <t>Fire Bolt</t>
-  </si>
-  <si>
-    <t>90% SP
-3 range</t>
-  </si>
-  <si>
     <t>Magic Arrow</t>
   </si>
   <si>
-    <t>75% SP + x
-4 range
-diagonally</t>
+    <t>100% SP, 3 range diagonally.
++50% damage to CC'ed</t>
+  </si>
+  <si>
+    <t>Siphon Mana</t>
+  </si>
+  <si>
+    <t>Drain up to 2 mana from a target.</t>
   </si>
   <si>
     <t>Blink</t>
   </si>
   <si>
     <t>Instant
-Teleport 2 range</t>
+Teleport 4 range</t>
+  </si>
+  <si>
+    <t>Iceberg Drop</t>
+  </si>
+  <si>
+    <t>Delayed 3x3
+165% SP
+Stuns targets</t>
   </si>
   <si>
     <t>Mana Ward</t>
@@ -3661,9 +3797,6 @@
   <si>
     <t>4 range
 75% SP health</t>
-  </si>
-  <si>
-    <t>Iceberg Drop</t>
   </si>
   <si>
     <t>40% SP
@@ -4006,10 +4139,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -4110,6 +4243,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -4120,21 +4267,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4143,6 +4276,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4195,23 +4335,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4225,7 +4365,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -4233,15 +4372,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4263,19 +4396,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4287,13 +4438,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4311,7 +4456,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4323,7 +4468,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4335,7 +4492,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4347,103 +4576,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4761,11 +4894,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4811,26 +4950,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4858,12 +4980,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4881,130 +5014,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6274,10 +6407,10 @@
   <sheetPr/>
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -6366,14 +6499,17 @@
       <c r="E3" s="23" t="s">
         <v>29</v>
       </c>
+      <c r="F3" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="I3" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N3"/>
     </row>
     <row r="4" ht="90" customHeight="1" spans="1:14">
       <c r="A4" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_6A82539A52A34473B077CC1FF6D19737",1)</f>
@@ -6383,19 +6519,19 @@
         <v>32</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="23" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N4"/>
     </row>
     <row r="5" ht="87" customHeight="1" spans="1:14">
       <c r="A5" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_0D1348BF351942C0B94814EB2E6C33B3",1)</f>
@@ -6405,25 +6541,25 @@
         <v>32</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N5"/>
     </row>
     <row r="6" ht="58" customHeight="1" spans="1:14">
       <c r="A6" s="23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_5DCB40CCA6B44244B7519B2BA06EDF1C",1)</f>
@@ -6436,16 +6572,16 @@
         <v>32</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N6"/>
     </row>
     <row r="7" ht="68" customHeight="1" spans="1:14">
       <c r="A7" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_48D844B5BD4E47F1A264B90859DAC1E8",1)</f>
@@ -6455,25 +6591,25 @@
         <v>32</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E7" s="23" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N7"/>
     </row>
     <row r="8" ht="71" customHeight="1" spans="1:14">
       <c r="A8" s="30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" s="31" t="str">
         <f>_xlfn.DISPIMG("ID_9997CD209D774EEAB420C53DDEA056A0",1)</f>
@@ -6483,22 +6619,22 @@
         <v>32</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N8"/>
     </row>
     <row r="9" ht="75" customHeight="1" spans="1:14">
       <c r="A9" s="23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B9" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_A28CCF741D2F4C959572208881E29708",1)</f>
@@ -6514,533 +6650,540 @@
         <v>29</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I9" s="24"/>
       <c r="N9"/>
     </row>
     <row r="10" ht="71" customHeight="1" spans="1:14">
       <c r="A10" s="23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_6763D977B250450ABFE5A7D8A1F632C1",1)</f>
         <v>=DISPIMG("ID_6763D977B250450ABFE5A7D8A1F632C1",1)</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>64</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G10" s="24"/>
       <c r="N10"/>
     </row>
-    <row r="11" ht="85" customHeight="1" spans="1:6">
+    <row r="11" ht="102" customHeight="1" spans="1:7">
       <c r="A11" s="23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B11" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_163A9240D4EF485292D7AE5FEFA9852F",1)</f>
         <v>=DISPIMG("ID_163A9240D4EF485292D7AE5FEFA9852F",1)</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" ht="75" customHeight="1" spans="1:14">
       <c r="A12" s="23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B12" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_7ED09DD668894ABE8A725CF2D4D0029F",1)</f>
         <v>=DISPIMG("ID_7ED09DD668894ABE8A725CF2D4D0029F",1)</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="N12"/>
     </row>
     <row r="13" ht="66" customHeight="1" spans="1:14">
       <c r="A13" s="23" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B13" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_D36F8EAEDC3D4A2D9DDF24AE96ABB005",1)</f>
         <v>=DISPIMG("ID_D36F8EAEDC3D4A2D9DDF24AE96ABB005",1)</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N13"/>
     </row>
     <row r="14" ht="75" customHeight="1" spans="1:14">
       <c r="A14" s="23" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B14" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_A046AFD9A3BF492EADA57F8350871DB2",1)</f>
         <v>=DISPIMG("ID_A046AFD9A3BF492EADA57F8350871DB2",1)</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N14"/>
     </row>
     <row r="15" ht="75" customHeight="1" spans="1:14">
       <c r="A15" s="23" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B15" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_2AC053A6DE184E4097DCE1BD0082E519",1)</f>
         <v>=DISPIMG("ID_2AC053A6DE184E4097DCE1BD0082E519",1)</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N15"/>
     </row>
     <row r="16" ht="75" customHeight="1" spans="1:14">
       <c r="A16" s="23" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B16" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_D72C5AF664FF4D6C8BB8BF8BE922256D",1)</f>
         <v>=DISPIMG("ID_D72C5AF664FF4D6C8BB8BF8BE922256D",1)</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="N16"/>
     </row>
     <row r="17" ht="75" customHeight="1" spans="1:14">
       <c r="A17" s="23" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B17" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_8F384D93F8A041A7BCCE76056201BF0F",1)</f>
         <v>=DISPIMG("ID_8F384D93F8A041A7BCCE76056201BF0F",1)</v>
       </c>
       <c r="C17" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>66</v>
-      </c>
       <c r="E17" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N17"/>
     </row>
     <row r="18" ht="75" customHeight="1" spans="1:14">
       <c r="A18" s="23" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B18" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_096FB0EDD1054600AEE93DB32445E432",1)</f>
         <v>=DISPIMG("ID_096FB0EDD1054600AEE93DB32445E432",1)</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="N18"/>
     </row>
     <row r="19" ht="75" customHeight="1" spans="1:14">
       <c r="A19" s="23" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B19" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_FD9E219F3F5B421E997BB811EC08D139",1)</f>
         <v>=DISPIMG("ID_FD9E219F3F5B421E997BB811EC08D139",1)</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="N19"/>
     </row>
     <row r="20" ht="75" customHeight="1" spans="1:14">
       <c r="A20" s="23" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B20" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_8A4C0CA2B27A4C878CAEF5F7F6D84956",1)</f>
         <v>=DISPIMG("ID_8A4C0CA2B27A4C878CAEF5F7F6D84956",1)</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="24" t="s">
-        <v>94</v>
-      </c>
       <c r="H20" s="24" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="N20"/>
     </row>
     <row r="21" ht="75" customHeight="1" spans="1:14">
       <c r="A21" s="23" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B21" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_F8B9634EB73D4F649475A0DA1DCAE550",1)</f>
         <v>=DISPIMG("ID_F8B9634EB73D4F649475A0DA1DCAE550",1)</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N21"/>
     </row>
     <row r="22" ht="45" customHeight="1" spans="1:14">
       <c r="A22" s="23" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B22" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_53946E75DFA2463A9C5A11C27661E786",1)</f>
         <v>=DISPIMG("ID_53946E75DFA2463A9C5A11C27661E786",1)</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="N22"/>
     </row>
     <row r="23" ht="75" customHeight="1" spans="1:14">
       <c r="A23" s="23" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B23" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_A9D352B95303458B89C1717F79CDE735",1)</f>
         <v>=DISPIMG("ID_A9D352B95303458B89C1717F79CDE735",1)</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="N23"/>
     </row>
     <row r="24" ht="75" customHeight="1" spans="1:14">
       <c r="A24" s="23" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B24" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_E06E036609E94BB9929FE03D33A7B60B",1)</f>
         <v>=DISPIMG("ID_E06E036609E94BB9929FE03D33A7B60B",1)</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F24" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" s="24" t="s">
         <v>114</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>111</v>
       </c>
       <c r="N24"/>
     </row>
     <row r="25" ht="75" customHeight="1" spans="1:14">
       <c r="A25" s="23" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B25" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_904652B47CF844A8B4968D95A64E3891",1)</f>
         <v>=DISPIMG("ID_904652B47CF844A8B4968D95A64E3891",1)</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="N25"/>
     </row>
     <row r="26" ht="75" customHeight="1" spans="1:14">
       <c r="A26" s="23" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B26" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_C711069D368A4C1E9B8B5E98151EADAC",1)</f>
         <v>=DISPIMG("ID_C711069D368A4C1E9B8B5E98151EADAC",1)</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="N26"/>
     </row>
     <row r="27" ht="75" customHeight="1" spans="1:14">
       <c r="A27" s="23" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B27" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_6C082183216B495085F7DBF1E3D99F5E",1)</f>
         <v>=DISPIMG("ID_6C082183216B495085F7DBF1E3D99F5E",1)</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N27"/>
     </row>
     <row r="28" ht="75" customHeight="1" spans="1:14">
       <c r="A28" s="23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B28" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_628E96F4BF42434FA277775E1DE2AA20",1)</f>
         <v>=DISPIMG("ID_628E96F4BF42434FA277775E1DE2AA20",1)</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="N28"/>
     </row>
     <row r="29" ht="75" customHeight="1" spans="1:14">
       <c r="A29" s="23" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B29" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_B9BED2D4AE354012A6BAB6A7E0FF5802",1)</f>
         <v>=DISPIMG("ID_B9BED2D4AE354012A6BAB6A7E0FF5802",1)</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N29"/>
     </row>
     <row r="30" ht="75" customHeight="1" spans="1:14">
       <c r="A30" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B30" s="31" t="str">
         <f>_xlfn.DISPIMG("ID_7A9E03A399CC4F74B895A88C9005BB92",1)</f>
         <v>=DISPIMG("ID_7A9E03A399CC4F74B895A88C9005BB92",1)</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N30"/>
     </row>
     <row r="31" ht="75" customHeight="1" spans="1:14">
       <c r="A31" s="23" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B31" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_65FDB7CD50CF472E9EE58BDBA9A1B3FA",1)</f>
         <v>=DISPIMG("ID_65FDB7CD50CF472E9EE58BDBA9A1B3FA",1)</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N31"/>
     </row>
@@ -7050,255 +7193,249 @@
     </row>
     <row r="33" ht="75" customHeight="1" spans="1:14">
       <c r="A33" s="23" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B33" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_AFFBB67C163A41AA92F2B00342A712D5",1)</f>
         <v>=DISPIMG("ID_AFFBB67C163A41AA92F2B00342A712D5",1)</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="N33"/>
     </row>
     <row r="34" ht="75" customHeight="1" spans="1:14">
       <c r="A34" s="23" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B34" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_A2CCFFC477CB41C68B5C4B028618A131",1)</f>
         <v>=DISPIMG("ID_A2CCFFC477CB41C68B5C4B028618A131",1)</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N34"/>
     </row>
     <row r="35" ht="75" customHeight="1" spans="1:14">
       <c r="A35" s="23" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B35" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_83BCD919FA48483A8504C30F86775227",1)</f>
         <v>=DISPIMG("ID_83BCD919FA48483A8504C30F86775227",1)</v>
       </c>
-      <c r="C35" s="23" t="s">
-        <v>108</v>
-      </c>
       <c r="F35" s="24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="N35"/>
     </row>
     <row r="36" ht="75" customHeight="1" spans="1:14">
       <c r="A36" s="23" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B36" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_F6C581482AFC49CF88B4B51DB4C2B884",1)</f>
         <v>=DISPIMG("ID_F6C581482AFC49CF88B4B51DB4C2B884",1)</v>
       </c>
-      <c r="C36" s="23" t="s">
-        <v>108</v>
-      </c>
       <c r="F36" s="24" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="N36"/>
     </row>
     <row r="37" ht="75" customHeight="1" spans="1:14">
       <c r="A37" s="23" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B37" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_B56FE51048C84C21B0544EC1D2B49BFB",1)</f>
         <v>=DISPIMG("ID_B56FE51048C84C21B0544EC1D2B49BFB",1)</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="N37"/>
     </row>
     <row r="38" ht="75" customHeight="1" spans="1:14">
       <c r="A38" s="23" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B38" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_2BF7160B000D4507A9BC6E9CD0CFBB9A",1)</f>
         <v>=DISPIMG("ID_2BF7160B000D4507A9BC6E9CD0CFBB9A",1)</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="N38"/>
     </row>
     <row r="39" ht="75" customHeight="1" spans="1:14">
       <c r="A39" s="23" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B39" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_F51C6D32B5FE4CB4BAE5E9D1DF1B99A4",1)</f>
         <v>=DISPIMG("ID_F51C6D32B5FE4CB4BAE5E9D1DF1B99A4",1)</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N39"/>
     </row>
     <row r="40" ht="75" customHeight="1" spans="1:14">
       <c r="A40" s="23" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B40" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_42E1FCCA38754E91AC4BDE1CCF581E79",1)</f>
         <v>=DISPIMG("ID_42E1FCCA38754E91AC4BDE1CCF581E79",1)</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H40" s="24" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="N40"/>
     </row>
     <row r="41" ht="75" customHeight="1" spans="1:14">
       <c r="A41" s="23" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B41" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_FCC8AFB7F83C4286AEE68D9A89ABD31C",1)</f>
         <v>=DISPIMG("ID_FCC8AFB7F83C4286AEE68D9A89ABD31C",1)</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="N41"/>
     </row>
     <row r="42" ht="75" customHeight="1" spans="1:14">
       <c r="A42" s="23" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B42" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_28ECA6BF9B5F4B8AB2A28048D7A7B8D6",1)</f>
         <v>=DISPIMG("ID_28ECA6BF9B5F4B8AB2A28048D7A7B8D6",1)</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="N42"/>
     </row>
     <row r="43" ht="75" customHeight="1" spans="1:14">
       <c r="A43" s="23" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B43" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_4F83562294774CE1B91320A1884FEEA6",1)</f>
         <v>=DISPIMG("ID_4F83562294774CE1B91320A1884FEEA6",1)</v>
       </c>
       <c r="F43" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="G43" s="24" t="s">
         <v>168</v>
-      </c>
-      <c r="G43" s="24" t="s">
-        <v>166</v>
       </c>
       <c r="N43"/>
     </row>
     <row r="44" ht="75" customHeight="1" spans="1:14">
       <c r="A44" s="23" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B44" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_50AEDFD4C9CB4FD09CD7DBAA4E44C1E5",1)</f>
         <v>=DISPIMG("ID_50AEDFD4C9CB4FD09CD7DBAA4E44C1E5",1)</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N44"/>
     </row>
     <row r="45" ht="75" customHeight="1" spans="1:14">
       <c r="A45" s="23" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B45" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_7FEFC25B5DDF45199372FEC1ECD4F0DB",1)</f>
         <v>=DISPIMG("ID_7FEFC25B5DDF45199372FEC1ECD4F0DB",1)</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J45" s="24" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="N45"/>
     </row>
     <row r="46" ht="75" customHeight="1" spans="1:14">
       <c r="A46" s="23" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B46" s="29" t="str">
         <f>_xlfn.DISPIMG("ID_563C63C9B19047BAA87384017A514719",1)</f>
         <v>=DISPIMG("ID_563C63C9B19047BAA87384017A514719",1)</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="N46"/>
     </row>
@@ -7308,22 +7445,22 @@
     </row>
     <row r="48" ht="75.75" spans="1:14">
       <c r="A48" s="23" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E48" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H48" s="33"/>
       <c r="I48" s="35"/>
@@ -7331,258 +7468,258 @@
     </row>
     <row r="49" ht="56.25" spans="1:14">
       <c r="A49" s="23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N49"/>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="23" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E50" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="N50"/>
     </row>
     <row r="51" ht="37.5" spans="1:14">
       <c r="A51" s="23" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E51" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="N51"/>
     </row>
     <row r="52" ht="56.25" spans="1:14">
       <c r="A52" s="23" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E52" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="N52"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" ht="56.25" spans="1:6">
       <c r="A54" s="23" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E54" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" ht="56.25" spans="1:8">
       <c r="A55" s="23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E55" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H55" s="24" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" ht="37.5" spans="1:8">
       <c r="A56" s="23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E56" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G56" s="24" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="H56" s="24" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" ht="37.5" spans="1:8">
       <c r="A57" s="23" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E57" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H57" s="24" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" ht="37.5" spans="1:7">
       <c r="A58" s="23" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E58" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" ht="56.25" spans="1:8">
       <c r="A59" s="23" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E59" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H59" s="24" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" ht="37.5" spans="1:13">
       <c r="A60" s="23" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E60" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G60" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K60" s="34" t="s">
         <v>7</v>
@@ -7596,22 +7733,22 @@
     </row>
     <row r="61" ht="56.25" spans="1:13">
       <c r="A61" s="23" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E61" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G61" s="24" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="K61" s="38">
         <v>1</v>
@@ -7625,25 +7762,25 @@
     </row>
     <row r="62" ht="37.5" spans="1:13">
       <c r="A62" s="23" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E62" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H62" s="24" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K62" s="38">
         <v>2</v>
@@ -7657,19 +7794,19 @@
     </row>
     <row r="63" ht="37.5" spans="1:13">
       <c r="A63" s="23" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K63" s="38">
         <v>3</v>
@@ -7683,19 +7820,19 @@
     </row>
     <row r="64" ht="56.25" spans="1:13">
       <c r="A64" s="23" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E64" s="24" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="K64" s="38">
         <v>4</v>
@@ -7709,25 +7846,25 @@
     </row>
     <row r="65" ht="37.5" spans="1:13">
       <c r="A65" s="23" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="K65" s="38">
         <v>5</v>
@@ -7741,19 +7878,19 @@
     </row>
     <row r="66" ht="37.5" spans="1:13">
       <c r="A66" s="23" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E66" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="K66" s="38">
         <v>6</v>
@@ -7767,7 +7904,7 @@
     </row>
     <row r="67" ht="37.5" spans="1:13">
       <c r="A67" s="24" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B67" s="24"/>
       <c r="K67" s="38">
@@ -7782,7 +7919,7 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="23" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="K68" s="38">
         <v>8</v>
@@ -7796,10 +7933,10 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="23" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="K69" s="38">
         <v>9</v>
@@ -7813,10 +7950,10 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="23" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="K70" s="41">
         <v>10</v>
@@ -7830,10 +7967,10 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="23" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -7868,37 +8005,37 @@
   <sheetData>
     <row r="3" spans="2:8">
       <c r="B3" s="14" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" ht="65.55" customHeight="1" spans="2:7">
       <c r="B4" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</f>
         <v>=DISPIMG("ID_1C66898D56284284A37A02A3EF585440",1)</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="G4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_2440730E3B794D249A4BBFB68234E0A5",1)</f>
@@ -7907,39 +8044,39 @@
     </row>
     <row r="5" ht="44" customHeight="1" spans="2:8">
       <c r="B5" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</f>
         <v>=DISPIMG("ID_922A22EB4F3240DF82F7BC8E2334A939",1)</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="G5" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</f>
         <v>=DISPIMG("ID_3FB322F6A35B4E67A56CEB159387F4E7",1)</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" ht="47" customHeight="1" spans="2:7">
       <c r="B6" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</f>
         <v>=DISPIMG("ID_6A4BCF7CF4234DD3963837ADFB704BB7",1)</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_491D9B3CF8B4441CAD720B86DCA07462",1)</f>
@@ -7948,39 +8085,39 @@
     </row>
     <row r="7" ht="64" customHeight="1" spans="2:8">
       <c r="B7" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</f>
         <v>=DISPIMG("ID_DCED4DA3234A4C4592F9A953085503D2",1)</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="G7" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</f>
         <v>=DISPIMG("ID_03A246FAB8D54EF0A611A5197A16854B",1)</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" ht="40" customHeight="1" spans="2:7">
       <c r="B8" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</f>
         <v>=DISPIMG("ID_E927AF64AF1F4F0796C389FC221298A8",1)</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="G8" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_DD37BC4AF6A646D482F166D1DA3483B9",1)</f>
@@ -7989,13 +8126,13 @@
     </row>
     <row r="9" ht="62" customHeight="1" spans="2:7">
       <c r="B9" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G9" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_CC66E0BDF222479FBCA1D73D9EEF98C9",1)</f>
@@ -8004,7 +8141,7 @@
     </row>
     <row r="10" ht="33" customHeight="1" spans="6:7">
       <c r="F10" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G10" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_69F91952F7254C9081725FDDC3777D6A",1)</f>
@@ -8013,14 +8150,14 @@
     </row>
     <row r="11" ht="50" customHeight="1" spans="6:8">
       <c r="F11" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G11" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</f>
         <v>=DISPIMG("ID_5883AB3B095E4C91BA3FA08ED96F1A98",1)</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -8032,10 +8169,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -8055,46 +8192,46 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="14" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>27</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" ht="44" customHeight="1" spans="2:10">
       <c r="B2" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C2" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B89FB7A8B8234D6EAF929FE5AE44207A",1)</f>
         <v>=DISPIMG("ID_B89FB7A8B8234D6EAF929FE5AE44207A",1)</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E2" s="1">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -8102,23 +8239,23 @@
     </row>
     <row r="3" ht="45" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</f>
         <v>=DISPIMG("ID_D90184E2EFC94DFCB03996685EEFC48E",1)</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E3" s="1">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="J3" s="1">
         <v>2</v>
@@ -8126,23 +8263,23 @@
     </row>
     <row r="4" ht="29.25" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_601DEB5433E749A5B04D3AB579BF0284",1)</f>
         <v>=DISPIMG("ID_601DEB5433E749A5B04D3AB579BF0284",1)</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -8150,17 +8287,17 @@
     </row>
     <row r="5" ht="117" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_435D6C639B07467EA8A5C2BDBADEB9EF",1)</f>
         <v>=DISPIMG("ID_435D6C639B07467EA8A5C2BDBADEB9EF",1)</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
@@ -8168,17 +8305,17 @@
     </row>
     <row r="6" ht="117" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_F93D45808FD1497AA14207AA5687A0B5",1)</f>
         <v>=DISPIMG("ID_F93D45808FD1497AA14207AA5687A0B5",1)</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
@@ -8186,128 +8323,128 @@
     </row>
     <row r="7" ht="61" customHeight="1" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_BD2F4EFF81EA407EB07B30FC9A025ED8",1)</f>
         <v>=DISPIMG("ID_BD2F4EFF81EA407EB07B30FC9A025ED8",1)</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" ht="56" customHeight="1" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_6F93A133E4B345C3A8C8AB0E41048D37",1)</f>
         <v>=DISPIMG("ID_6F93A133E4B345C3A8C8AB0E41048D37",1)</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" ht="67" customHeight="1" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_9DE1483F06B1441B9301F11BB84D2728",1)</f>
         <v>=DISPIMG("ID_9DE1483F06B1441B9301F11BB84D2728",1)</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" ht="97" customHeight="1" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_E2D7BCC771AE4C57B67785698BAAC802",1)</f>
         <v>=DISPIMG("ID_E2D7BCC771AE4C57B67785698BAAC802",1)</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" ht="80" customHeight="1" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_068CF9D1A64D4B1AA847F491190CA498",1)</f>
         <v>=DISPIMG("ID_068CF9D1A64D4B1AA847F491190CA498",1)</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" ht="67" customHeight="1" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B819211F6D714CDEBBF38A9148AFAAC7",1)</f>
         <v>=DISPIMG("ID_B819211F6D714CDEBBF38A9148AFAAC7",1)</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" ht="69" customHeight="1" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_0D3B38AE54A44B3E8DF025084DB6651B",1)</f>
         <v>=DISPIMG("ID_0D3B38AE54A44B3E8DF025084DB6651B",1)</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" ht="71" customHeight="1" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</f>
         <v>=DISPIMG("ID_797F597F1B7F46D7BFE49889C122C20E",1)</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E14" s="1">
         <v>6</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="J14" s="1">
         <v>5</v>
@@ -8315,23 +8452,23 @@
     </row>
     <row r="15" ht="93.75" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_900DEDBC95DA49B6832F8E0EAF3922E7",1)</f>
         <v>=DISPIMG("ID_900DEDBC95DA49B6832F8E0EAF3922E7",1)</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E15" s="1">
         <v>5</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="J15" s="1">
         <v>6</v>
@@ -8339,83 +8476,83 @@
     </row>
     <row r="16" ht="117" customHeight="1" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_F1C740FD556749E1A3007CADB7F7B5AD",1)</f>
         <v>=DISPIMG("ID_F1C740FD556749E1A3007CADB7F7B5AD",1)</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="17" ht="53" customHeight="1" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_7295A5EE838846E9918EEC2351B4AADE",1)</f>
         <v>=DISPIMG("ID_7295A5EE838846E9918EEC2351B4AADE",1)</v>
       </c>
       <c r="D17" s="70" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" ht="70" customHeight="1" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_475395F073B348EBAD90A05DB4F70535",1)</f>
         <v>=DISPIMG("ID_475395F073B348EBAD90A05DB4F70535",1)</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="19" ht="37.5" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</f>
         <v>=DISPIMG("ID_6D29D48731D64D15B7AFC6A55F3580E6",1)</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" ht="37.5" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_5B5C76B37B874958A231351EBD5A6E7C",1)</f>
         <v>=DISPIMG("ID_5B5C76B37B874958A231351EBD5A6E7C",1)</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E20" s="1">
         <v>5</v>
@@ -8423,17 +8560,17 @@
     </row>
     <row r="21" ht="75" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B7F3E8AB96A746EEA8D18747E89057C6",1)</f>
         <v>=DISPIMG("ID_B7F3E8AB96A746EEA8D18747E89057C6",1)</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E21" s="1">
         <v>5</v>
@@ -8441,17 +8578,17 @@
     </row>
     <row r="22" ht="37.5" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C22" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_52D5A41E637044A490A457D53A6E6968",1)</f>
         <v>=DISPIMG("ID_52D5A41E637044A490A457D53A6E6968",1)</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E22" s="1">
         <v>8</v>
@@ -8459,17 +8596,17 @@
     </row>
     <row r="23" ht="93.75" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3B6DDDD98A8F40BC81817AB7D481E31C",1)</f>
         <v>=DISPIMG("ID_3B6DDDD98A8F40BC81817AB7D481E31C",1)</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -8477,17 +8614,17 @@
     </row>
     <row r="24" ht="56.25" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_9DEEB880DCB04491A4378D1013CB4998",1)</f>
         <v>=DISPIMG("ID_9DEEB880DCB04491A4378D1013CB4998",1)</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E24" s="1">
         <v>4</v>
@@ -8498,17 +8635,17 @@
     </row>
     <row r="25" ht="75" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</f>
         <v>=DISPIMG("ID_937E3FF1032A441DAFCEF81E0E8651CE",1)</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E25" s="1">
         <v>3</v>
@@ -8519,17 +8656,17 @@
     </row>
     <row r="26" ht="86" customHeight="1" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C26" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_FB929A3456EC484B83246B63E363119F",1)</f>
         <v>=DISPIMG("ID_FB929A3456EC484B83246B63E363119F",1)</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -8537,17 +8674,17 @@
     </row>
     <row r="27" ht="74" customHeight="1" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C27" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_CDF4F9B6AAE7428396B6B6CB350938A4",1)</f>
         <v>=DISPIMG("ID_CDF4F9B6AAE7428396B6B6CB350938A4",1)</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E27" s="1">
         <v>8</v>
@@ -8558,17 +8695,17 @@
     </row>
     <row r="28" ht="98" customHeight="1" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C28" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_9E20CD0B9D3344AFA01653BE39E9CAED",1)</f>
         <v>=DISPIMG("ID_9E20CD0B9D3344AFA01653BE39E9CAED",1)</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E28" s="1">
         <v>4</v>
@@ -8576,56 +8713,56 @@
     </row>
     <row r="29" ht="29.25" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C29" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_05B2EF6AB8B64DED9EE5B9B0C23F991B",1)</f>
         <v>=DISPIMG("ID_05B2EF6AB8B64DED9EE5B9B0C23F991B",1)</v>
       </c>
       <c r="D29" s="71" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" ht="44" customHeight="1" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C30" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_B70ADECACB0640B388DDE4A570E8A4A0",1)</f>
         <v>=DISPIMG("ID_B70ADECACB0640B388DDE4A570E8A4A0",1)</v>
       </c>
       <c r="D30" s="70" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="31" ht="93.75" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C31" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_F991DDDB9E524EFEA1B831F26AB76DE9",1)</f>
         <v>=DISPIMG("ID_F991DDDB9E524EFEA1B831F26AB76DE9",1)</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -8633,332 +8770,352 @@
     </row>
     <row r="32" ht="37.5" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C32" s="1" t="str">
         <f>_xlfn.DISPIMG("ID_3597ED710A4940C9B87FCDF5F4476A1D",1)</f>
         <v>=DISPIMG("ID_3597ED710A4940C9B87FCDF5F4476A1D",1)</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="33" ht="39" customHeight="1" spans="1:6">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33" ht="50" customHeight="1" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
+      </c>
+      <c r="C33" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_BB4C04DA0D82463FB165645D87472EF4",1)</f>
+        <v>=DISPIMG("ID_BB4C04DA0D82463FB165645D87472EF4",1)</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="34" ht="37.5" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
+      </c>
+      <c r="C34" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_38F9D2AF49AB4BCA9F11DD0853E30AF5",1)</f>
+        <v>=DISPIMG("ID_38F9D2AF49AB4BCA9F11DD0853E30AF5",1)</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="E34" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" ht="37" customHeight="1" spans="1:5">
+      <c r="A35" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="E34" s="1">
+      <c r="B35" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C35" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_36828F0C21034B8DBBF17DCCDA5DA267",1)</f>
+        <v>=DISPIMG("ID_36828F0C21034B8DBBF17DCCDA5DA267",1)</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E35" s="1">
         <v>0</v>
-      </c>
-    </row>
-    <row r="35" ht="56.25" spans="1:5">
-      <c r="A35" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="E35" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="36" ht="37.5" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
+      </c>
+      <c r="C36" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_A9DB86C046194BD7BA43F0E79E4830FA",1)</f>
+        <v>=DISPIMG("ID_A9DB86C046194BD7BA43F0E79E4830FA",1)</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E36" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="37" ht="56.25" spans="1:5">
+    <row r="37" ht="37" customHeight="1" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
+      </c>
+      <c r="C37" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_8658678BBB954416846A781790E04465",1)</f>
+        <v>=DISPIMG("ID_8658678BBB954416846A781790E04465",1)</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="E37" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="38" ht="75" spans="1:5">
+    <row r="38" ht="56.25" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E38" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" ht="75" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>371</v>
       </c>
       <c r="E39" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="40" ht="56.25" spans="1:5">
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>373</v>
       </c>
       <c r="E40" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" ht="37.5" spans="1:5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" ht="56.25" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E41" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="42" ht="56.25" spans="1:5">
+    <row r="42" ht="37.5" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>374</v>
+        <v>359</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>376</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E42" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" ht="56.25" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E43" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="43" ht="75" spans="1:4">
-      <c r="A43" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>376</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+    <row r="44" ht="75" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D44" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>379</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>379</v>
+      <c r="D44" s="3" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>285</v>
+        <v>381</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E45" s="1">
+        <v>382</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E46" s="1">
         <v>0</v>
-      </c>
-    </row>
-    <row r="46" ht="37.5" spans="1:5">
-      <c r="A46" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="E46" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="47" ht="37.5" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" ht="37.5" spans="1:5">
+      <c r="A48" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="E47" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" ht="75" spans="1:5">
-      <c r="A48" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="B48" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E48" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="49" ht="93.75" spans="1:5">
+    <row r="49" ht="75" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E49" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" ht="93.75" spans="1:5">
+      <c r="A50" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="E50" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="51" ht="75" spans="1:5">
+    <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>390</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="E51" s="1">
+        <v>383</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="52" ht="75" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E52" s="1">
         <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="54" ht="56.25" spans="1:5">
-      <c r="A54" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>394</v>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>395</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="E54" s="1">
-        <v>5</v>
+        <v>382</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="55" ht="56.25" spans="1:5">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>396</v>
       </c>
       <c r="B55" s="20" t="s">
@@ -8971,7 +9128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" ht="37.5" spans="1:5">
+    <row r="56" ht="56.25" spans="1:5">
       <c r="A56" s="1" t="s">
         <v>399</v>
       </c>
@@ -8982,10 +9139,10 @@
         <v>401</v>
       </c>
       <c r="E56" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" ht="75" spans="1:5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" ht="37.5" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>402</v>
       </c>
@@ -8996,26 +9153,26 @@
         <v>404</v>
       </c>
       <c r="E57" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" ht="75" spans="1:5">
+      <c r="A58" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>406</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E58" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="58" ht="56.25" spans="1:5">
-      <c r="A58" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="B58" s="20" t="s">
-        <v>405</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="E58" s="1">
-        <v>4</v>
-      </c>
-    </row>
     <row r="59" ht="56.25" spans="1:5">
-      <c r="A59" s="3" t="s">
-        <v>407</v>
+      <c r="A59" s="1" t="s">
+        <v>399</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>408</v>
@@ -9024,11 +9181,11 @@
         <v>409</v>
       </c>
       <c r="E59" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" ht="56.25" spans="1:5">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>410</v>
       </c>
       <c r="B60" s="20" t="s">
@@ -9041,23 +9198,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" ht="37.5" spans="1:5">
+    <row r="61" ht="56.25" spans="1:5">
       <c r="A61" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="B61" s="19" t="s">
         <v>413</v>
       </c>
+      <c r="B61" s="20" t="s">
+        <v>414</v>
+      </c>
       <c r="D61" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="62" ht="56.25" spans="1:5">
-      <c r="A62" s="3" t="s">
         <v>415</v>
+      </c>
+      <c r="E61" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" ht="37.5" spans="1:5">
+      <c r="A62" s="1" t="s">
+        <v>355</v>
       </c>
       <c r="B62" s="19" t="s">
         <v>416</v>
@@ -9066,18 +9223,32 @@
         <v>417</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="63" ht="56.25" spans="1:4">
-      <c r="A63" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="63" ht="56.25" spans="1:5">
+      <c r="A63" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="19" t="s">
         <v>419</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>420</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="64" ht="56.25" spans="1:4">
+      <c r="A64" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -9112,7 +9283,7 @@
   <sheetData>
     <row r="2" ht="30" customHeight="1" spans="2:6">
       <c r="B2" s="4" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -9121,73 +9292,73 @@
     </row>
     <row r="3" ht="38.25" spans="2:4">
       <c r="B3" s="7" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" ht="57" spans="2:6">
       <c r="B4" s="8" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" ht="38.25" spans="2:6">
       <c r="B5" s="2" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" ht="84" customHeight="1" spans="2:6">
       <c r="B6" s="2" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" ht="19.5" spans="2:10">
       <c r="B8" s="9" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -9200,28 +9371,28 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="D9" s="1">
         <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="10" ht="38.25" spans="2:7">
@@ -9229,19 +9400,19 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -9274,13 +9445,13 @@
   <sheetData>
     <row r="2" ht="81" customHeight="1" spans="2:4">
       <c r="B2" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for 2022-05-16. Too many updates to count. See discord.
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -2391,11 +2391,236 @@
       </xdr:spPr>
     </xdr:pic>
   </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="95" name="ID_19D2822555484122B1A19AE87FFD1927" descr="S_Axe06"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId94"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3006725" y="30086300"/>
+          <a:ext cx="323215" cy="323215"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="96" name="ID_DEBA4EF89213482E8901533D1E663720" descr="Ice Cube"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId95"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3097530" y="30817185"/>
+          <a:ext cx="303530" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="97" name="ID_78111E53C0A24E34802FBAA95F98312C" descr="Ignite"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId96"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3097530" y="31609030"/>
+          <a:ext cx="304165" cy="301625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="98" name="ID_C45D4AF5D4FB4FF6801F8DE1A2A665B5" descr="Frost Nova"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId97"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3064510" y="32445960"/>
+          <a:ext cx="303530" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="99" name="ID_66DABD3D114D4ED1889A2F8B72197191" descr="S_Physic01"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId98"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2981325" y="32247205"/>
+          <a:ext cx="427355" cy="431800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="100" name="ID_41280E9E4E9A4CA7A4C14BD14E0E85CE" descr="Very Magic Arrow"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId99"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3122295" y="34122360"/>
+          <a:ext cx="303530" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="101" name="ID_2F3AB0F4F76E4A7F89B7B19D6534EE66" descr="Shocking Startup"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId100"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3081020" y="34876740"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="102" name="ID_4A43E83676EA4DAA893ABC1CBA6011E0" descr="Momentum Magic"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId101"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3105785" y="35497135"/>
+          <a:ext cx="303530" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
+  <etc:cellImage>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="103" name="ID_94307C1A67984EFF9A26A73E0F27F702" descr="Everblocker"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId102"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3106420" y="36019105"/>
+          <a:ext cx="304165" cy="309245"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+  </etc:cellImage>
 </etc:cellImages>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="472">
   <si>
     <t>Player Level</t>
   </si>
@@ -3769,6 +3994,60 @@
 85% SP + 20% max mana</t>
   </si>
   <si>
+    <t>Ice Cube</t>
+  </si>
+  <si>
+    <t>Conjure an ice cube :3</t>
+  </si>
+  <si>
+    <t>Ignite</t>
+  </si>
+  <si>
+    <t>All enemies bleed</t>
+  </si>
+  <si>
+    <t>Obstacle Focus</t>
+  </si>
+  <si>
+    <t>Choose an obstacle.
+AoE around it.
+Effect depends on material.</t>
+  </si>
+  <si>
+    <t>Frost Nova</t>
+  </si>
+  <si>
+    <t>50% SP around and root.
+If already rooted, 100% SP
+and stun.</t>
+  </si>
+  <si>
+    <t>Very Magic Arrow</t>
+  </si>
+  <si>
+    <t>Magic arrow becomes usable
+in a straight line too.</t>
+  </si>
+  <si>
+    <t>Shocking Startup</t>
+  </si>
+  <si>
+    <t>At combat start, damage random
+enemy for 10 SHOCK damage.</t>
+  </si>
+  <si>
+    <t>Momentum Magic</t>
+  </si>
+  <si>
+    <t>Any spell cast = +1 SP until turn end</t>
+  </si>
+  <si>
+    <t>Everblocker</t>
+  </si>
+  <si>
+    <t>Any spell cast = 1 BLOCK</t>
+  </si>
+  <si>
     <t>Ice Spike</t>
   </si>
   <si>
@@ -3778,12 +4057,6 @@
 in a straight line</t>
   </si>
   <si>
-    <t>Ignite</t>
-  </si>
-  <si>
-    <t>All enemies bleed</t>
-  </si>
-  <si>
     <t>Slowdown</t>
   </si>
   <si>
@@ -3797,11 +4070,6 @@
   <si>
     <t>4 range
 75% SP health</t>
-  </si>
-  <si>
-    <t>40% SP
-4 range (TIR)
-Stuns the target</t>
   </si>
   <si>
     <t>Soul Drain</t>
@@ -4139,10 +4407,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -4243,6 +4511,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -4257,32 +4540,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4297,6 +4565,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -4304,15 +4580,8 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -4327,14 +4596,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -4342,11 +4603,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4366,7 +4626,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4380,8 +4640,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4396,97 +4664,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4504,7 +4688,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4516,7 +4772,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4528,25 +4790,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4558,25 +4808,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4894,21 +5162,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -4958,6 +5211,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -4974,15 +5242,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -4991,20 +5250,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -5014,130 +5282,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6678,7 +6946,6 @@
       <c r="F10" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="24"/>
       <c r="N10"/>
     </row>
     <row r="11" ht="102" customHeight="1" spans="1:7">
@@ -8169,10 +8436,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -8886,6 +9153,10 @@
       <c r="B38" s="1" t="s">
         <v>368</v>
       </c>
+      <c r="C38" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_19D2822555484122B1A19AE87FFD1927",1)</f>
+        <v>=DISPIMG("ID_19D2822555484122B1A19AE87FFD1927",1)</v>
+      </c>
       <c r="D38" s="3" t="s">
         <v>369</v>
       </c>
@@ -8893,27 +9164,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" ht="75" spans="1:5">
+    <row r="39" ht="63" customHeight="1" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>359</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>370</v>
       </c>
+      <c r="C39" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_DEBA4EF89213482E8901533D1E663720",1)</f>
+        <v>=DISPIMG("ID_DEBA4EF89213482E8901533D1E663720",1)</v>
+      </c>
       <c r="D39" s="3" t="s">
         <v>371</v>
       </c>
       <c r="E39" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" ht="60" customHeight="1" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>359</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>372</v>
       </c>
+      <c r="C40" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_78111E53C0A24E34802FBAA95F98312C",1)</f>
+        <v>=DISPIMG("ID_78111E53C0A24E34802FBAA95F98312C",1)</v>
+      </c>
       <c r="D40" s="1" t="s">
         <v>373</v>
       </c>
@@ -8921,334 +9200,446 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" ht="56.25" spans="1:5">
+    <row r="41" ht="60" customHeight="1" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>359</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>374</v>
       </c>
+      <c r="C41" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_66DABD3D114D4ED1889A2F8B72197191",1)</f>
+        <v>=DISPIMG("ID_66DABD3D114D4ED1889A2F8B72197191",1)</v>
+      </c>
       <c r="D41" s="3" t="s">
         <v>375</v>
       </c>
       <c r="E41" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" ht="37.5" spans="1:5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" ht="74" customHeight="1" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>359</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>376</v>
       </c>
+      <c r="C42" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_C45D4AF5D4FB4FF6801F8DE1A2A665B5",1)</f>
+        <v>=DISPIMG("ID_C45D4AF5D4FB4FF6801F8DE1A2A665B5",1)</v>
+      </c>
       <c r="D42" s="3" t="s">
         <v>377</v>
       </c>
       <c r="E42" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" ht="56.25" spans="1:5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" ht="62" customHeight="1" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>366</v>
+      <c r="B43" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_41280E9E4E9A4CA7A4C14BD14E0E85CE",1)</f>
+        <v>=DISPIMG("ID_41280E9E4E9A4CA7A4C14BD14E0E85CE",1)</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="E43" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" ht="75" spans="1:4">
+        <v>379</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="44" ht="58" customHeight="1" spans="1:5">
       <c r="A44" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>379</v>
+      <c r="B44" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_2F3AB0F4F76E4A7F89B7B19D6534EE66",1)</f>
+        <v>=DISPIMG("ID_2F3AB0F4F76E4A7F89B7B19D6534EE66",1)</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>381</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="45" ht="45" customHeight="1" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>359</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D45" s="1" t="s">
         <v>382</v>
       </c>
+      <c r="C45" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_4A43E83676EA4DAA893ABC1CBA6011E0",1)</f>
+        <v>=DISPIMG("ID_4A43E83676EA4DAA893ABC1CBA6011E0",1)</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>383</v>
+      </c>
       <c r="E45" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="46" ht="46" customHeight="1" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E46" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" ht="37.5" spans="1:5">
+        <v>384</v>
+      </c>
+      <c r="C46" s="1" t="str">
+        <f>_xlfn.DISPIMG("ID_94307C1A67984EFF9A26A73E0F27F702",1)</f>
+        <v>=DISPIMG("ID_94307C1A67984EFF9A26A73E0F27F702",1)</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="47" ht="75" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E47" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" ht="37.5" spans="1:5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" ht="56.25" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E48" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="49" ht="75" spans="1:5">
+    <row r="49" ht="37.5" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E49" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="50" ht="93.75" spans="1:5">
-      <c r="A50" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="E50" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+    <row r="50" spans="2:4">
+      <c r="B50" s="19"/>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" ht="75" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="B51" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>392</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="52" ht="75" spans="1:5">
+      <c r="D51" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="D52" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="E52" s="1">
-        <v>4</v>
+      <c r="D52" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>287</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" ht="37.5" spans="1:5">
       <c r="A54" s="1" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="55" ht="56.25" spans="1:5">
-      <c r="A55" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="E54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" ht="37.5" spans="1:5">
+      <c r="A55" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B55" s="20" t="s">
-        <v>397</v>
+      <c r="B55" s="1" t="s">
+        <v>399</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E55" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" ht="56.25" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" ht="75" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>400</v>
+        <v>396</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>401</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E56" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" ht="37.5" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" ht="93.75" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B57" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>403</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>404</v>
       </c>
       <c r="E57" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" ht="75" spans="1:5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="D58" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="59" ht="75" spans="1:5">
+      <c r="A59" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>406</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="E58" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" ht="56.25" spans="1:5">
-      <c r="A59" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="B59" s="20" t="s">
-        <v>408</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>409</v>
       </c>
       <c r="E59" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="60" ht="56.25" spans="1:5">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="62" ht="56.25" spans="1:5">
+      <c r="A62" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B62" s="20" t="s">
         <v>410</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="D62" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="E62" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" ht="56.25" spans="1:5">
+      <c r="A63" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="E60" s="1">
+      <c r="B63" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="E63" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" ht="37.5" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="E64" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="61" ht="56.25" spans="1:5">
-      <c r="A61" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="B61" s="20" t="s">
-        <v>414</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="E61" s="1">
+    <row r="65" ht="75" spans="1:5">
+      <c r="A65" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="E65" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" ht="56.25" spans="1:5">
+      <c r="A66" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>421</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="E66" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" ht="56.25" spans="1:5">
+      <c r="A67" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="E67" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="62" ht="37.5" spans="1:5">
-      <c r="A62" s="1" t="s">
+    <row r="68" ht="56.25" spans="1:5">
+      <c r="A68" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="E68" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" ht="37.5" spans="1:5">
+      <c r="A69" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="B62" s="19" t="s">
-        <v>416</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="E62" s="1" t="s">
+      <c r="B69" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="63" ht="56.25" spans="1:5">
-      <c r="A63" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="B63" s="19" t="s">
-        <v>419</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="E63" s="1" t="s">
+    <row r="70" ht="56.25" spans="1:5">
+      <c r="A70" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>432</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="64" ht="56.25" spans="1:4">
-      <c r="A64" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>423</v>
+    <row r="71" ht="56.25" spans="1:4">
+      <c r="A71" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -9283,7 +9674,7 @@
   <sheetData>
     <row r="2" ht="30" customHeight="1" spans="2:6">
       <c r="B2" s="4" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -9292,73 +9683,73 @@
     </row>
     <row r="3" ht="38.25" spans="2:4">
       <c r="B3" s="7" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" ht="57" spans="2:6">
       <c r="B4" s="8" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>429</v>
+        <v>442</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>432</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" ht="38.25" spans="2:6">
       <c r="B5" s="2" t="s">
-        <v>433</v>
+        <v>446</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>434</v>
+        <v>447</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" ht="84" customHeight="1" spans="2:6">
       <c r="B6" s="2" t="s">
-        <v>436</v>
+        <v>449</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>438</v>
+        <v>451</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>439</v>
+        <v>452</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" ht="19.5" spans="2:10">
       <c r="B8" s="9" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -9371,28 +9762,28 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>445</v>
+        <v>458</v>
       </c>
       <c r="D9" s="1">
         <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" ht="38.25" spans="2:7">
@@ -9400,19 +9791,19 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>454</v>
+        <v>467</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>455</v>
+        <v>468</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>456</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -9448,10 +9839,10 @@
         <v>293</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>457</v>
+        <v>470</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>458</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added plenty of polishing. AfterCombat screen now displays all items with multiple popups. Added cooldown timer UI's to spells.
</commit_message>
<xml_diff>
--- a/Design Tables.xlsx
+++ b/Design Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23295" windowHeight="13095" activeTab="3"/>
+    <workbookView windowWidth="24225" windowHeight="12045" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Stats" sheetId="1" r:id="rId1"/>
@@ -4407,10 +4407,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -4511,30 +4511,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4548,9 +4526,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4565,6 +4589,21 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -4572,32 +4611,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4610,31 +4625,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4654,6 +4647,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -4664,7 +4664,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4676,7 +4694,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4688,19 +4760,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4712,73 +4802,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4796,55 +4826,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5162,6 +5162,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -5242,17 +5253,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -5264,7 +5264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5282,130 +5282,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -8439,7 +8439,7 @@
   <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>

</xml_diff>